<commit_message>
first review of the entire workflow
</commit_message>
<xml_diff>
--- a/data/RLIe_scores.xlsx
+++ b/data/RLIe_scores.xlsx
@@ -531,7 +531,7 @@
         <v>0.34</v>
       </c>
       <c r="G5">
-        <v>0.8</v>
+        <v>0.78</v>
       </c>
       <c r="H5" t="inlineStr">
         <is>
@@ -563,7 +563,7 @@
         <v>0.9090909090909091</v>
       </c>
       <c r="F6">
-        <v>0.8361363636363638</v>
+        <v>0.8363636363636364</v>
       </c>
       <c r="G6">
         <v>0.9727272727272728</v>
@@ -843,10 +843,10 @@
         <v>0.6481203007518797</v>
       </c>
       <c r="F14">
-        <v>0.5864661654135339</v>
+        <v>0.5834586466165413</v>
       </c>
       <c r="G14">
-        <v>0.7082706766917293</v>
+        <v>0.7097744360902256</v>
       </c>
       <c r="H14" t="inlineStr">
         <is>
@@ -913,7 +913,7 @@
         <v>0.6330827067669174</v>
       </c>
       <c r="F16">
-        <v>0.5699248120300752</v>
+        <v>0.5714285714285714</v>
       </c>
       <c r="G16">
         <v>0.6947368421052631</v>
@@ -948,10 +948,10 @@
         <v>0.6330827067669174</v>
       </c>
       <c r="F17">
-        <v>0.5698872180451128</v>
+        <v>0.5714285714285714</v>
       </c>
       <c r="G17">
-        <v>0.6962406015037594</v>
+        <v>0.6947368421052631</v>
       </c>
       <c r="H17" t="inlineStr">
         <is>
@@ -983,10 +983,10 @@
         <v>0.87</v>
       </c>
       <c r="F18">
-        <v>0.8322222222222222</v>
+        <v>0.8333333333333334</v>
       </c>
       <c r="G18">
-        <v>0.9033333333333333</v>
+        <v>0.9055555555555556</v>
       </c>
       <c r="H18" t="inlineStr">
         <is>
@@ -1018,10 +1018,10 @@
         <v>0.8455555555555556</v>
       </c>
       <c r="F19">
-        <v>0.8077777777777778</v>
+        <v>0.8044444444444444</v>
       </c>
       <c r="G19">
-        <v>0.8844444444444445</v>
+        <v>0.8822222222222222</v>
       </c>
       <c r="H19" t="inlineStr">
         <is>
@@ -1053,7 +1053,7 @@
         <v>0.8388888888888889</v>
       </c>
       <c r="F20">
-        <v>0.7988888888888889</v>
+        <v>0.7977777777777778</v>
       </c>
       <c r="G20">
         <v>0.8766666666666667</v>
@@ -1088,10 +1088,10 @@
         <v>0.8344444444444444</v>
       </c>
       <c r="F21">
-        <v>0.7933333333333333</v>
+        <v>0.7944444444444445</v>
       </c>
       <c r="G21">
-        <v>0.8744444444444445</v>
+        <v>0.8733333333333333</v>
       </c>
       <c r="H21" t="inlineStr">
         <is>
@@ -1123,7 +1123,7 @@
         <v>0.9369565217391305</v>
       </c>
       <c r="F22">
-        <v>0.8913043478260869</v>
+        <v>0.8934782608695653</v>
       </c>
       <c r="G22">
         <v>0.9760869565217392</v>
@@ -1161,7 +1161,7 @@
         <v>0.8695652173913043</v>
       </c>
       <c r="G23">
-        <v>0.9630434782608696</v>
+        <v>0.9652173913043478</v>
       </c>
       <c r="H23" t="inlineStr">
         <is>
@@ -1193,10 +1193,10 @@
         <v>0.9195652173913044</v>
       </c>
       <c r="F24">
-        <v>0.8673913043478261</v>
+        <v>0.8695652173913043</v>
       </c>
       <c r="G24">
-        <v>0.9630434782608696</v>
+        <v>0.9673913043478261</v>
       </c>
       <c r="H24" t="inlineStr">
         <is>
@@ -1228,7 +1228,7 @@
         <v>0.9195652173913044</v>
       </c>
       <c r="F25">
-        <v>0.8717391304347826</v>
+        <v>0.8673913043478261</v>
       </c>
       <c r="G25">
         <v>0.9630434782608696</v>
@@ -1301,7 +1301,7 @@
         <v>0.34</v>
       </c>
       <c r="G27">
-        <v>0.78</v>
+        <v>0.8</v>
       </c>
       <c r="H27" t="inlineStr">
         <is>
@@ -1403,7 +1403,7 @@
         <v>0.9090909090909091</v>
       </c>
       <c r="F30">
-        <v>0.8363636363636364</v>
+        <v>0.8272727272727273</v>
       </c>
       <c r="G30">
         <v>0.9727272727272728</v>
@@ -1826,7 +1826,7 @@
         <v>0.5833333333333333</v>
       </c>
       <c r="G42">
-        <v>0.7060984848484843</v>
+        <v>0.7075757575757575</v>
       </c>
       <c r="H42" t="inlineStr">
         <is>
@@ -1861,7 +1861,7 @@
         <v>0.5681818181818181</v>
       </c>
       <c r="G43">
-        <v>0.6924242424242424</v>
+        <v>0.6909469696969691</v>
       </c>
       <c r="H43" t="inlineStr">
         <is>
@@ -1896,7 +1896,7 @@
         <v>0.5681818181818181</v>
       </c>
       <c r="G44">
-        <v>0.693939393939394</v>
+        <v>0.6924242424242424</v>
       </c>
       <c r="H44" t="inlineStr">
         <is>
@@ -1931,7 +1931,7 @@
         <v>0.5666666666666667</v>
       </c>
       <c r="G45">
-        <v>0.693939393939394</v>
+        <v>0.6924242424242424</v>
       </c>
       <c r="H45" t="inlineStr">
         <is>
@@ -1963,7 +1963,7 @@
         <v>0.9421052631578948</v>
       </c>
       <c r="F46">
-        <v>0.8789473684210526</v>
+        <v>0.8842105263157894</v>
       </c>
       <c r="G46">
         <v>0.9894736842105263</v>
@@ -1998,7 +1998,7 @@
         <v>0.9421052631578948</v>
       </c>
       <c r="F47">
-        <v>0.8789473684210526</v>
+        <v>0.8842105263157894</v>
       </c>
       <c r="G47">
         <v>0.9894736842105263</v>
@@ -2033,7 +2033,7 @@
         <v>0.9263157894736842</v>
       </c>
       <c r="F48">
-        <v>0.8631578947368421</v>
+        <v>0.8578947368421053</v>
       </c>
       <c r="G48">
         <v>0.9842105263157894</v>
@@ -2068,7 +2068,7 @@
         <v>0.9263157894736842</v>
       </c>
       <c r="F49">
-        <v>0.8578947368421053</v>
+        <v>0.8630263157894738</v>
       </c>
       <c r="G49">
         <v>0.9842105263157894</v>
@@ -2106,7 +2106,7 @@
         <v>0.7820895522388059</v>
       </c>
       <c r="G50">
-        <v>0.9104477611940298</v>
+        <v>0.9105223880597004</v>
       </c>
       <c r="H50" t="inlineStr">
         <is>
@@ -2138,7 +2138,7 @@
         <v>0.8149253731343283</v>
       </c>
       <c r="F51">
-        <v>0.7462686567164178</v>
+        <v>0.7432835820895523</v>
       </c>
       <c r="G51">
         <v>0.8805970149253731</v>
@@ -2176,7 +2176,7 @@
         <v>0.7343283582089553</v>
       </c>
       <c r="G52">
-        <v>0.8716417910447761</v>
+        <v>0.8746268656716418</v>
       </c>
       <c r="H52" t="inlineStr">
         <is>
@@ -2211,7 +2211,7 @@
         <v>0.7343283582089553</v>
       </c>
       <c r="G53">
-        <v>0.8776119402985074</v>
+        <v>0.8746268656716418</v>
       </c>
       <c r="H53" t="inlineStr">
         <is>
@@ -2281,7 +2281,7 @@
         <v>0.76</v>
       </c>
       <c r="G55">
-        <v>0.8853333333333333</v>
+        <v>0.8826666666666667</v>
       </c>
       <c r="H55" t="inlineStr">
         <is>
@@ -2348,7 +2348,7 @@
         <v>0.8133333333333334</v>
       </c>
       <c r="F57">
-        <v>0.7493333333333334</v>
+        <v>0.7466666666666666</v>
       </c>
       <c r="G57">
         <v>0.8773333333333333</v>
@@ -2526,7 +2526,7 @@
         <v>0.8603174603174604</v>
       </c>
       <c r="G62">
-        <v>0.9682539682539683</v>
+        <v>0.9746031746031746</v>
       </c>
       <c r="H62" t="inlineStr">
         <is>
@@ -2593,7 +2593,7 @@
         <v>0.9079365079365079</v>
       </c>
       <c r="F64">
-        <v>0.8412698412698413</v>
+        <v>0.8444444444444444</v>
       </c>
       <c r="G64">
         <v>0.9650793650793651</v>
@@ -2798,10 +2798,10 @@
         <v>0.8215982721382289</v>
       </c>
       <c r="F70">
-        <v>0.7939524838012959</v>
+        <v>0.7935205183585313</v>
       </c>
       <c r="G70">
-        <v>0.8475161987041037</v>
+        <v>0.8488120950323974</v>
       </c>
       <c r="H70" t="inlineStr">
         <is>
@@ -2828,10 +2828,10 @@
         <v>0.7987041036717063</v>
       </c>
       <c r="F71">
-        <v>0.7706155507559395</v>
+        <v>0.7688876889848812</v>
       </c>
       <c r="G71">
-        <v>0.8272138228941684</v>
+        <v>0.8267926565874728</v>
       </c>
       <c r="H71" t="inlineStr">
         <is>
@@ -2861,7 +2861,7 @@
         <v>0.767170626349892</v>
       </c>
       <c r="G72">
-        <v>0.824622030237581</v>
+        <v>0.8241900647948164</v>
       </c>
       <c r="H72" t="inlineStr">
         <is>
@@ -2888,7 +2888,7 @@
         <v>0.7943844492440605</v>
       </c>
       <c r="F73">
-        <v>0.7654427645788338</v>
+        <v>0.7645788336933046</v>
       </c>
       <c r="G73">
         <v>0.8228941684665227</v>

</xml_diff>

<commit_message>
updates RLIe figures and gitignore
</commit_message>
<xml_diff>
--- a/data/RLIe_scores.xlsx
+++ b/data/RLIe_scores.xlsx
@@ -461,7 +461,7 @@
         <v>0.34</v>
       </c>
       <c r="G3">
-        <v>0.78</v>
+        <v>0.8</v>
       </c>
       <c r="H3" t="inlineStr">
         <is>
@@ -563,7 +563,7 @@
         <v>0.9090909090909091</v>
       </c>
       <c r="F6">
-        <v>0.8363636363636364</v>
+        <v>0.8272727272727273</v>
       </c>
       <c r="G6">
         <v>0.9727272727272728</v>
@@ -843,7 +843,7 @@
         <v>0.6481203007518797</v>
       </c>
       <c r="F14">
-        <v>0.5834586466165413</v>
+        <v>0.5864661654135339</v>
       </c>
       <c r="G14">
         <v>0.7097744360902256</v>
@@ -878,10 +878,10 @@
         <v>0.6330827067669174</v>
       </c>
       <c r="F15">
-        <v>0.5699248120300752</v>
+        <v>0.5714285714285714</v>
       </c>
       <c r="G15">
-        <v>0.6947368421052631</v>
+        <v>0.6962406015037594</v>
       </c>
       <c r="H15" t="inlineStr">
         <is>
@@ -913,10 +913,10 @@
         <v>0.6330827067669174</v>
       </c>
       <c r="F16">
-        <v>0.5714285714285714</v>
+        <v>0.5699248120300752</v>
       </c>
       <c r="G16">
-        <v>0.6947368421052631</v>
+        <v>0.693233082706767</v>
       </c>
       <c r="H16" t="inlineStr">
         <is>
@@ -948,10 +948,10 @@
         <v>0.6330827067669174</v>
       </c>
       <c r="F17">
-        <v>0.5714285714285714</v>
+        <v>0.5699248120300752</v>
       </c>
       <c r="G17">
-        <v>0.6947368421052631</v>
+        <v>0.693233082706767</v>
       </c>
       <c r="H17" t="inlineStr">
         <is>
@@ -1021,7 +1021,7 @@
         <v>0.8044444444444444</v>
       </c>
       <c r="G19">
-        <v>0.8822222222222222</v>
+        <v>0.8833333333333333</v>
       </c>
       <c r="H19" t="inlineStr">
         <is>
@@ -1053,10 +1053,10 @@
         <v>0.8388888888888889</v>
       </c>
       <c r="F20">
-        <v>0.7977777777777778</v>
+        <v>0.8</v>
       </c>
       <c r="G20">
-        <v>0.8766666666666667</v>
+        <v>0.8777777777777778</v>
       </c>
       <c r="H20" t="inlineStr">
         <is>
@@ -1088,7 +1088,7 @@
         <v>0.8344444444444444</v>
       </c>
       <c r="F21">
-        <v>0.7944444444444445</v>
+        <v>0.7933333333333333</v>
       </c>
       <c r="G21">
         <v>0.8733333333333333</v>
@@ -1123,7 +1123,7 @@
         <v>0.9369565217391305</v>
       </c>
       <c r="F22">
-        <v>0.8934782608695653</v>
+        <v>0.8913043478260869</v>
       </c>
       <c r="G22">
         <v>0.9760869565217392</v>
@@ -1196,7 +1196,7 @@
         <v>0.8695652173913043</v>
       </c>
       <c r="G24">
-        <v>0.9673913043478261</v>
+        <v>0.9652173913043478</v>
       </c>
       <c r="H24" t="inlineStr">
         <is>
@@ -1228,7 +1228,7 @@
         <v>0.9195652173913044</v>
       </c>
       <c r="F25">
-        <v>0.8673913043478261</v>
+        <v>0.8695652173913043</v>
       </c>
       <c r="G25">
         <v>0.9630434782608696</v>
@@ -1263,7 +1263,7 @@
         <v>0.74</v>
       </c>
       <c r="F26">
-        <v>0.54</v>
+        <v>0.52</v>
       </c>
       <c r="G26">
         <v>0.9399999999999999</v>
@@ -1301,7 +1301,7 @@
         <v>0.34</v>
       </c>
       <c r="G27">
-        <v>0.8</v>
+        <v>0.78</v>
       </c>
       <c r="H27" t="inlineStr">
         <is>
@@ -1371,7 +1371,7 @@
         <v>0.34</v>
       </c>
       <c r="G29">
-        <v>0.78</v>
+        <v>0.7804999999999928</v>
       </c>
       <c r="H29" t="inlineStr">
         <is>
@@ -1403,7 +1403,7 @@
         <v>0.9090909090909091</v>
       </c>
       <c r="F30">
-        <v>0.8272727272727273</v>
+        <v>0.8363636363636364</v>
       </c>
       <c r="G30">
         <v>0.9727272727272728</v>
@@ -1823,10 +1823,10 @@
         <v>0.6454545454545455</v>
       </c>
       <c r="F42">
-        <v>0.5833333333333333</v>
+        <v>0.5848484848484848</v>
       </c>
       <c r="G42">
-        <v>0.7075757575757575</v>
+        <v>0.7060606060606061</v>
       </c>
       <c r="H42" t="inlineStr">
         <is>
@@ -1858,10 +1858,10 @@
         <v>0.6303030303030304</v>
       </c>
       <c r="F43">
-        <v>0.5681818181818181</v>
+        <v>0.5666666666666667</v>
       </c>
       <c r="G43">
-        <v>0.6909469696969691</v>
+        <v>0.693939393939394</v>
       </c>
       <c r="H43" t="inlineStr">
         <is>
@@ -1893,7 +1893,7 @@
         <v>0.6303030303030304</v>
       </c>
       <c r="F44">
-        <v>0.5681818181818181</v>
+        <v>0.5696969696969697</v>
       </c>
       <c r="G44">
         <v>0.6924242424242424</v>
@@ -1928,10 +1928,10 @@
         <v>0.6303030303030304</v>
       </c>
       <c r="F45">
-        <v>0.5666666666666667</v>
+        <v>0.5681818181818181</v>
       </c>
       <c r="G45">
-        <v>0.6924242424242424</v>
+        <v>0.6909090909090909</v>
       </c>
       <c r="H45" t="inlineStr">
         <is>
@@ -2033,7 +2033,7 @@
         <v>0.9263157894736842</v>
       </c>
       <c r="F48">
-        <v>0.8578947368421053</v>
+        <v>0.8631578947368421</v>
       </c>
       <c r="G48">
         <v>0.9842105263157894</v>
@@ -2068,7 +2068,7 @@
         <v>0.9263157894736842</v>
       </c>
       <c r="F49">
-        <v>0.8630263157894738</v>
+        <v>0.8578947368421053</v>
       </c>
       <c r="G49">
         <v>0.9842105263157894</v>
@@ -2106,7 +2106,7 @@
         <v>0.7820895522388059</v>
       </c>
       <c r="G50">
-        <v>0.9105223880597004</v>
+        <v>0.9134328358208955</v>
       </c>
       <c r="H50" t="inlineStr">
         <is>
@@ -2173,10 +2173,10 @@
         <v>0.8059701492537313</v>
       </c>
       <c r="F52">
-        <v>0.7343283582089553</v>
+        <v>0.7313432835820896</v>
       </c>
       <c r="G52">
-        <v>0.8746268656716418</v>
+        <v>0.8716417910447761</v>
       </c>
       <c r="H52" t="inlineStr">
         <is>
@@ -2211,7 +2211,7 @@
         <v>0.7343283582089553</v>
       </c>
       <c r="G53">
-        <v>0.8746268656716418</v>
+        <v>0.8716417910447761</v>
       </c>
       <c r="H53" t="inlineStr">
         <is>
@@ -2243,7 +2243,7 @@
         <v>0.8506666666666667</v>
       </c>
       <c r="F54">
-        <v>0.792</v>
+        <v>0.7893333333333333</v>
       </c>
       <c r="G54">
         <v>0.9066666666666666</v>
@@ -2278,10 +2278,10 @@
         <v>0.8240000000000001</v>
       </c>
       <c r="F55">
-        <v>0.76</v>
+        <v>0.7573333333333333</v>
       </c>
       <c r="G55">
-        <v>0.8826666666666667</v>
+        <v>0.8853333333333333</v>
       </c>
       <c r="H55" t="inlineStr">
         <is>
@@ -2313,10 +2313,10 @@
         <v>0.8240000000000001</v>
       </c>
       <c r="F56">
-        <v>0.76</v>
+        <v>0.7626666666666666</v>
       </c>
       <c r="G56">
-        <v>0.8826666666666667</v>
+        <v>0.8853333333333333</v>
       </c>
       <c r="H56" t="inlineStr">
         <is>
@@ -2351,7 +2351,7 @@
         <v>0.7466666666666666</v>
       </c>
       <c r="G57">
-        <v>0.8773333333333333</v>
+        <v>0.8746666666666667</v>
       </c>
       <c r="H57" t="inlineStr">
         <is>
@@ -2596,7 +2596,7 @@
         <v>0.8444444444444444</v>
       </c>
       <c r="G64">
-        <v>0.9650793650793651</v>
+        <v>0.9619841269841258</v>
       </c>
       <c r="H64" t="inlineStr">
         <is>
@@ -2628,7 +2628,7 @@
         <v>0.9079365079365079</v>
       </c>
       <c r="F65">
-        <v>0.8444444444444444</v>
+        <v>0.8476190476190476</v>
       </c>
       <c r="G65">
         <v>0.9650793650793651</v>
@@ -2798,10 +2798,10 @@
         <v>0.8215982721382289</v>
       </c>
       <c r="F70">
-        <v>0.7935205183585313</v>
+        <v>0.7943844492440605</v>
       </c>
       <c r="G70">
-        <v>0.8488120950323974</v>
+        <v>0.849244060475162</v>
       </c>
       <c r="H70" t="inlineStr">
         <is>
@@ -2828,10 +2828,10 @@
         <v>0.7987041036717063</v>
       </c>
       <c r="F71">
-        <v>0.7688876889848812</v>
+        <v>0.7693304535637149</v>
       </c>
       <c r="G71">
-        <v>0.8267926565874728</v>
+        <v>0.827645788336933</v>
       </c>
       <c r="H71" t="inlineStr">
         <is>
@@ -2861,7 +2861,7 @@
         <v>0.767170626349892</v>
       </c>
       <c r="G72">
-        <v>0.8241900647948164</v>
+        <v>0.8250539956803455</v>
       </c>
       <c r="H72" t="inlineStr">
         <is>
@@ -2888,7 +2888,7 @@
         <v>0.7943844492440605</v>
       </c>
       <c r="F73">
-        <v>0.7645788336933046</v>
+        <v>0.7649999999999999</v>
       </c>
       <c r="G73">
         <v>0.8228941684665227</v>

</xml_diff>

<commit_message>
updated the bootstrap section
</commit_message>
<xml_diff>
--- a/data/RLIe_scores.xlsx
+++ b/data/RLIe_scores.xlsx
@@ -461,7 +461,7 @@
         <v>0.34</v>
       </c>
       <c r="G3">
-        <v>0.8</v>
+        <v>0.78</v>
       </c>
       <c r="H3" t="inlineStr">
         <is>
@@ -563,7 +563,7 @@
         <v>0.9090909090909091</v>
       </c>
       <c r="F6">
-        <v>0.8272727272727273</v>
+        <v>0.8363636363636364</v>
       </c>
       <c r="G6">
         <v>0.9727272727272728</v>
@@ -846,7 +846,7 @@
         <v>0.5864661654135339</v>
       </c>
       <c r="G14">
-        <v>0.7097744360902256</v>
+        <v>0.7098120300751876</v>
       </c>
       <c r="H14" t="inlineStr">
         <is>
@@ -913,10 +913,10 @@
         <v>0.6330827067669174</v>
       </c>
       <c r="F16">
-        <v>0.5699248120300752</v>
+        <v>0.5729323308270677</v>
       </c>
       <c r="G16">
-        <v>0.693233082706767</v>
+        <v>0.6962406015037594</v>
       </c>
       <c r="H16" t="inlineStr">
         <is>
@@ -948,10 +948,10 @@
         <v>0.6330827067669174</v>
       </c>
       <c r="F17">
-        <v>0.5699248120300752</v>
+        <v>0.5714285714285714</v>
       </c>
       <c r="G17">
-        <v>0.693233082706767</v>
+        <v>0.6977443609022556</v>
       </c>
       <c r="H17" t="inlineStr">
         <is>
@@ -983,10 +983,10 @@
         <v>0.87</v>
       </c>
       <c r="F18">
-        <v>0.8333333333333334</v>
+        <v>0.8322222222222222</v>
       </c>
       <c r="G18">
-        <v>0.9055555555555556</v>
+        <v>0.9044444444444444</v>
       </c>
       <c r="H18" t="inlineStr">
         <is>
@@ -1018,10 +1018,10 @@
         <v>0.8455555555555556</v>
       </c>
       <c r="F19">
-        <v>0.8044444444444444</v>
+        <v>0.8066666666666666</v>
       </c>
       <c r="G19">
-        <v>0.8833333333333333</v>
+        <v>0.8844444444444445</v>
       </c>
       <c r="H19" t="inlineStr">
         <is>
@@ -1053,7 +1053,7 @@
         <v>0.8388888888888889</v>
       </c>
       <c r="F20">
-        <v>0.8</v>
+        <v>0.7988611111111111</v>
       </c>
       <c r="G20">
         <v>0.8777777777777778</v>
@@ -1088,10 +1088,10 @@
         <v>0.8344444444444444</v>
       </c>
       <c r="F21">
-        <v>0.7933333333333333</v>
+        <v>0.7955555555555556</v>
       </c>
       <c r="G21">
-        <v>0.8733333333333333</v>
+        <v>0.8744444444444445</v>
       </c>
       <c r="H21" t="inlineStr">
         <is>
@@ -1231,7 +1231,7 @@
         <v>0.8695652173913043</v>
       </c>
       <c r="G25">
-        <v>0.9630434782608696</v>
+        <v>0.9630978260869557</v>
       </c>
       <c r="H25" t="inlineStr">
         <is>
@@ -1371,7 +1371,7 @@
         <v>0.34</v>
       </c>
       <c r="G29">
-        <v>0.7804999999999928</v>
+        <v>0.78</v>
       </c>
       <c r="H29" t="inlineStr">
         <is>
@@ -1403,7 +1403,7 @@
         <v>0.9090909090909091</v>
       </c>
       <c r="F30">
-        <v>0.8363636363636364</v>
+        <v>0.8272727272727273</v>
       </c>
       <c r="G30">
         <v>0.9727272727272728</v>
@@ -1441,7 +1441,7 @@
         <v>0.8090909090909091</v>
       </c>
       <c r="G31">
-        <v>0.9636363636363636</v>
+        <v>0.9545454545454546</v>
       </c>
       <c r="H31" t="inlineStr">
         <is>
@@ -1508,7 +1508,7 @@
         <v>0.8909090909090909</v>
       </c>
       <c r="F33">
-        <v>0.8090909090909091</v>
+        <v>0.8181818181818181</v>
       </c>
       <c r="G33">
         <v>0.9636363636363636</v>
@@ -1823,7 +1823,7 @@
         <v>0.6454545454545455</v>
       </c>
       <c r="F42">
-        <v>0.5848484848484848</v>
+        <v>0.5833333333333333</v>
       </c>
       <c r="G42">
         <v>0.7060606060606061</v>
@@ -1861,7 +1861,7 @@
         <v>0.5666666666666667</v>
       </c>
       <c r="G43">
-        <v>0.693939393939394</v>
+        <v>0.6909090909090909</v>
       </c>
       <c r="H43" t="inlineStr">
         <is>
@@ -1893,10 +1893,10 @@
         <v>0.6303030303030304</v>
       </c>
       <c r="F44">
-        <v>0.5696969696969697</v>
+        <v>0.5681818181818181</v>
       </c>
       <c r="G44">
-        <v>0.6924242424242424</v>
+        <v>0.6909090909090909</v>
       </c>
       <c r="H44" t="inlineStr">
         <is>
@@ -1963,7 +1963,7 @@
         <v>0.9421052631578948</v>
       </c>
       <c r="F46">
-        <v>0.8842105263157894</v>
+        <v>0.8789473684210526</v>
       </c>
       <c r="G46">
         <v>0.9894736842105263</v>
@@ -1998,7 +1998,7 @@
         <v>0.9421052631578948</v>
       </c>
       <c r="F47">
-        <v>0.8842105263157894</v>
+        <v>0.8789473684210526</v>
       </c>
       <c r="G47">
         <v>0.9894736842105263</v>
@@ -2068,7 +2068,7 @@
         <v>0.9263157894736842</v>
       </c>
       <c r="F49">
-        <v>0.8578947368421053</v>
+        <v>0.8631578947368421</v>
       </c>
       <c r="G49">
         <v>0.9842105263157894</v>
@@ -2103,7 +2103,7 @@
         <v>0.8507462686567164</v>
       </c>
       <c r="F50">
-        <v>0.7820895522388059</v>
+        <v>0.7850746268656716</v>
       </c>
       <c r="G50">
         <v>0.9134328358208955</v>
@@ -2138,7 +2138,7 @@
         <v>0.8149253731343283</v>
       </c>
       <c r="F51">
-        <v>0.7432835820895523</v>
+        <v>0.7462686567164178</v>
       </c>
       <c r="G51">
         <v>0.8805970149253731</v>
@@ -2173,10 +2173,10 @@
         <v>0.8059701492537313</v>
       </c>
       <c r="F52">
-        <v>0.7313432835820896</v>
+        <v>0.7343283582089553</v>
       </c>
       <c r="G52">
-        <v>0.8716417910447761</v>
+        <v>0.8746268656716418</v>
       </c>
       <c r="H52" t="inlineStr">
         <is>
@@ -2211,7 +2211,7 @@
         <v>0.7343283582089553</v>
       </c>
       <c r="G53">
-        <v>0.8716417910447761</v>
+        <v>0.8746268656716418</v>
       </c>
       <c r="H53" t="inlineStr">
         <is>
@@ -2243,10 +2243,10 @@
         <v>0.8506666666666667</v>
       </c>
       <c r="F54">
-        <v>0.7893333333333333</v>
+        <v>0.792</v>
       </c>
       <c r="G54">
-        <v>0.9066666666666666</v>
+        <v>0.904</v>
       </c>
       <c r="H54" t="inlineStr">
         <is>
@@ -2278,7 +2278,7 @@
         <v>0.8240000000000001</v>
       </c>
       <c r="F55">
-        <v>0.7573333333333333</v>
+        <v>0.7626666666666666</v>
       </c>
       <c r="G55">
         <v>0.8853333333333333</v>
@@ -2313,7 +2313,7 @@
         <v>0.8240000000000001</v>
       </c>
       <c r="F56">
-        <v>0.7626666666666666</v>
+        <v>0.76</v>
       </c>
       <c r="G56">
         <v>0.8853333333333333</v>
@@ -2348,7 +2348,7 @@
         <v>0.8133333333333334</v>
       </c>
       <c r="F57">
-        <v>0.7466666666666666</v>
+        <v>0.7493333333333334</v>
       </c>
       <c r="G57">
         <v>0.8746666666666667</v>
@@ -2558,7 +2558,7 @@
         <v>0.9079365079365079</v>
       </c>
       <c r="F63">
-        <v>0.8444444444444444</v>
+        <v>0.8412698412698413</v>
       </c>
       <c r="G63">
         <v>0.9650793650793651</v>
@@ -2596,7 +2596,7 @@
         <v>0.8444444444444444</v>
       </c>
       <c r="G64">
-        <v>0.9619841269841258</v>
+        <v>0.9650793650793651</v>
       </c>
       <c r="H64" t="inlineStr">
         <is>
@@ -2628,7 +2628,7 @@
         <v>0.9079365079365079</v>
       </c>
       <c r="F65">
-        <v>0.8476190476190476</v>
+        <v>0.8412698412698413</v>
       </c>
       <c r="G65">
         <v>0.9650793650793651</v>
@@ -2798,7 +2798,7 @@
         <v>0.8215982721382289</v>
       </c>
       <c r="F70">
-        <v>0.7943844492440605</v>
+        <v>0.7930885529157667</v>
       </c>
       <c r="G70">
         <v>0.849244060475162</v>
@@ -2828,10 +2828,10 @@
         <v>0.7987041036717063</v>
       </c>
       <c r="F71">
-        <v>0.7693304535637149</v>
+        <v>0.7697624190064795</v>
       </c>
       <c r="G71">
-        <v>0.827645788336933</v>
+        <v>0.8267818574514039</v>
       </c>
       <c r="H71" t="inlineStr">
         <is>
@@ -2888,10 +2888,10 @@
         <v>0.7943844492440605</v>
       </c>
       <c r="F73">
-        <v>0.7649999999999999</v>
+        <v>0.7650107991360691</v>
       </c>
       <c r="G73">
-        <v>0.8228941684665227</v>
+        <v>0.8220302375809936</v>
       </c>
       <c r="H73" t="inlineStr">
         <is>

</xml_diff>

<commit_message>
full GET text of the L2 and L3 codes
</commit_message>
<xml_diff>
--- a/data/RLIe_scores.xlsx
+++ b/data/RLIe_scores.xlsx
@@ -407,7 +407,7 @@
     <row r="2">
       <c r="A2" t="inlineStr">
         <is>
-          <t>MT2</t>
+          <t>MT2 : Supralittoral coastal systems</t>
         </is>
       </c>
       <c r="B2">
@@ -442,7 +442,7 @@
     <row r="3">
       <c r="A3" t="inlineStr">
         <is>
-          <t>MT2</t>
+          <t>MT2 : Supralittoral coastal systems</t>
         </is>
       </c>
       <c r="B3">
@@ -477,7 +477,7 @@
     <row r="4">
       <c r="A4" t="inlineStr">
         <is>
-          <t>MT2</t>
+          <t>MT2 : Supralittoral coastal systems</t>
         </is>
       </c>
       <c r="B4">
@@ -512,7 +512,7 @@
     <row r="5">
       <c r="A5" t="inlineStr">
         <is>
-          <t>MT2</t>
+          <t>MT2 : Supralittoral coastal systems</t>
         </is>
       </c>
       <c r="B5">
@@ -531,7 +531,7 @@
         <v>0.34</v>
       </c>
       <c r="G5">
-        <v>0.78</v>
+        <v>0.8</v>
       </c>
       <c r="H5" t="inlineStr">
         <is>
@@ -547,7 +547,7 @@
     <row r="6">
       <c r="A6" t="inlineStr">
         <is>
-          <t>T1</t>
+          <t>T1 : Tropical-subtropical forests</t>
         </is>
       </c>
       <c r="B6">
@@ -563,7 +563,7 @@
         <v>0.9090909090909091</v>
       </c>
       <c r="F6">
-        <v>0.8363636363636364</v>
+        <v>0.8272727272727273</v>
       </c>
       <c r="G6">
         <v>0.9727272727272728</v>
@@ -582,7 +582,7 @@
     <row r="7">
       <c r="A7" t="inlineStr">
         <is>
-          <t>T1</t>
+          <t>T1 : Tropical-subtropical forests</t>
         </is>
       </c>
       <c r="B7">
@@ -617,7 +617,7 @@
     <row r="8">
       <c r="A8" t="inlineStr">
         <is>
-          <t>T1</t>
+          <t>T1 : Tropical-subtropical forests</t>
         </is>
       </c>
       <c r="B8">
@@ -652,7 +652,7 @@
     <row r="9">
       <c r="A9" t="inlineStr">
         <is>
-          <t>T1</t>
+          <t>T1 : Tropical-subtropical forests</t>
         </is>
       </c>
       <c r="B9">
@@ -687,7 +687,7 @@
     <row r="10">
       <c r="A10" t="inlineStr">
         <is>
-          <t>T2</t>
+          <t>T2 : Temperate-boreal forests &amp; woodlands</t>
         </is>
       </c>
       <c r="B10">
@@ -722,7 +722,7 @@
     <row r="11">
       <c r="A11" t="inlineStr">
         <is>
-          <t>T2</t>
+          <t>T2 : Temperate-boreal forests &amp; woodlands</t>
         </is>
       </c>
       <c r="B11">
@@ -757,7 +757,7 @@
     <row r="12">
       <c r="A12" t="inlineStr">
         <is>
-          <t>T2</t>
+          <t>T2 : Temperate-boreal forests &amp; woodlands</t>
         </is>
       </c>
       <c r="B12">
@@ -792,7 +792,7 @@
     <row r="13">
       <c r="A13" t="inlineStr">
         <is>
-          <t>T2</t>
+          <t>T2 : Temperate-boreal forests &amp; woodlands</t>
         </is>
       </c>
       <c r="B13">
@@ -827,7 +827,7 @@
     <row r="14">
       <c r="A14" t="inlineStr">
         <is>
-          <t>T3</t>
+          <t>T3 : Shrublands &amp; shrubby woodlands</t>
         </is>
       </c>
       <c r="B14">
@@ -843,10 +843,10 @@
         <v>0.6481203007518797</v>
       </c>
       <c r="F14">
-        <v>0.5864661654135339</v>
+        <v>0.58796992481203</v>
       </c>
       <c r="G14">
-        <v>0.7098120300751876</v>
+        <v>0.7082706766917293</v>
       </c>
       <c r="H14" t="inlineStr">
         <is>
@@ -862,7 +862,7 @@
     <row r="15">
       <c r="A15" t="inlineStr">
         <is>
-          <t>T3</t>
+          <t>T3 : Shrublands &amp; shrubby woodlands</t>
         </is>
       </c>
       <c r="B15">
@@ -878,10 +878,10 @@
         <v>0.6330827067669174</v>
       </c>
       <c r="F15">
-        <v>0.5714285714285714</v>
+        <v>0.5684210526315789</v>
       </c>
       <c r="G15">
-        <v>0.6962406015037594</v>
+        <v>0.693233082706767</v>
       </c>
       <c r="H15" t="inlineStr">
         <is>
@@ -897,7 +897,7 @@
     <row r="16">
       <c r="A16" t="inlineStr">
         <is>
-          <t>T3</t>
+          <t>T3 : Shrublands &amp; shrubby woodlands</t>
         </is>
       </c>
       <c r="B16">
@@ -913,10 +913,10 @@
         <v>0.6330827067669174</v>
       </c>
       <c r="F16">
-        <v>0.5729323308270677</v>
+        <v>0.5684210526315789</v>
       </c>
       <c r="G16">
-        <v>0.6962406015037594</v>
+        <v>0.693233082706767</v>
       </c>
       <c r="H16" t="inlineStr">
         <is>
@@ -932,7 +932,7 @@
     <row r="17">
       <c r="A17" t="inlineStr">
         <is>
-          <t>T3</t>
+          <t>T3 : Shrublands &amp; shrubby woodlands</t>
         </is>
       </c>
       <c r="B17">
@@ -951,7 +951,7 @@
         <v>0.5714285714285714</v>
       </c>
       <c r="G17">
-        <v>0.6977443609022556</v>
+        <v>0.6962406015037594</v>
       </c>
       <c r="H17" t="inlineStr">
         <is>
@@ -967,7 +967,7 @@
     <row r="18">
       <c r="A18" t="inlineStr">
         <is>
-          <t>T4</t>
+          <t>T4 : Savannas and grasslands</t>
         </is>
       </c>
       <c r="B18">
@@ -983,7 +983,7 @@
         <v>0.87</v>
       </c>
       <c r="F18">
-        <v>0.8322222222222222</v>
+        <v>0.8344444444444444</v>
       </c>
       <c r="G18">
         <v>0.9044444444444444</v>
@@ -1002,7 +1002,7 @@
     <row r="19">
       <c r="A19" t="inlineStr">
         <is>
-          <t>T4</t>
+          <t>T4 : Savannas and grasslands</t>
         </is>
       </c>
       <c r="B19">
@@ -1018,10 +1018,10 @@
         <v>0.8455555555555556</v>
       </c>
       <c r="F19">
-        <v>0.8066666666666666</v>
+        <v>0.8055277777777778</v>
       </c>
       <c r="G19">
-        <v>0.8844444444444445</v>
+        <v>0.8833333333333333</v>
       </c>
       <c r="H19" t="inlineStr">
         <is>
@@ -1037,7 +1037,7 @@
     <row r="20">
       <c r="A20" t="inlineStr">
         <is>
-          <t>T4</t>
+          <t>T4 : Savannas and grasslands</t>
         </is>
       </c>
       <c r="B20">
@@ -1053,7 +1053,7 @@
         <v>0.8388888888888889</v>
       </c>
       <c r="F20">
-        <v>0.7988611111111111</v>
+        <v>0.7977777777777778</v>
       </c>
       <c r="G20">
         <v>0.8777777777777778</v>
@@ -1072,7 +1072,7 @@
     <row r="21">
       <c r="A21" t="inlineStr">
         <is>
-          <t>T4</t>
+          <t>T4 : Savannas and grasslands</t>
         </is>
       </c>
       <c r="B21">
@@ -1088,10 +1088,10 @@
         <v>0.8344444444444444</v>
       </c>
       <c r="F21">
-        <v>0.7955555555555556</v>
+        <v>0.7933333333333333</v>
       </c>
       <c r="G21">
-        <v>0.8744444444444445</v>
+        <v>0.8722222222222222</v>
       </c>
       <c r="H21" t="inlineStr">
         <is>
@@ -1107,7 +1107,7 @@
     <row r="22">
       <c r="A22" t="inlineStr">
         <is>
-          <t>T5</t>
+          <t>T5 : Deserts and semi-deserts</t>
         </is>
       </c>
       <c r="B22">
@@ -1142,7 +1142,7 @@
     <row r="23">
       <c r="A23" t="inlineStr">
         <is>
-          <t>T5</t>
+          <t>T5 : Deserts and semi-deserts</t>
         </is>
       </c>
       <c r="B23">
@@ -1161,7 +1161,7 @@
         <v>0.8695652173913043</v>
       </c>
       <c r="G23">
-        <v>0.9652173913043478</v>
+        <v>0.9630434782608696</v>
       </c>
       <c r="H23" t="inlineStr">
         <is>
@@ -1177,7 +1177,7 @@
     <row r="24">
       <c r="A24" t="inlineStr">
         <is>
-          <t>T5</t>
+          <t>T5 : Deserts and semi-deserts</t>
         </is>
       </c>
       <c r="B24">
@@ -1196,7 +1196,7 @@
         <v>0.8695652173913043</v>
       </c>
       <c r="G24">
-        <v>0.9652173913043478</v>
+        <v>0.9630434782608696</v>
       </c>
       <c r="H24" t="inlineStr">
         <is>
@@ -1212,7 +1212,7 @@
     <row r="25">
       <c r="A25" t="inlineStr">
         <is>
-          <t>T5</t>
+          <t>T5 : Deserts and semi-deserts</t>
         </is>
       </c>
       <c r="B25">
@@ -1228,10 +1228,10 @@
         <v>0.9195652173913044</v>
       </c>
       <c r="F25">
-        <v>0.8695652173913043</v>
+        <v>0.8673913043478261</v>
       </c>
       <c r="G25">
-        <v>0.9630978260869557</v>
+        <v>0.9652173913043478</v>
       </c>
       <c r="H25" t="inlineStr">
         <is>
@@ -1247,7 +1247,7 @@
     <row r="26">
       <c r="A26" t="inlineStr">
         <is>
-          <t>MT2.1</t>
+          <t>MT2.1 : Coastal shrublands and grasslands</t>
         </is>
       </c>
       <c r="B26">
@@ -1263,7 +1263,7 @@
         <v>0.74</v>
       </c>
       <c r="F26">
-        <v>0.52</v>
+        <v>0.54</v>
       </c>
       <c r="G26">
         <v>0.9399999999999999</v>
@@ -1282,7 +1282,7 @@
     <row r="27">
       <c r="A27" t="inlineStr">
         <is>
-          <t>MT2.1</t>
+          <t>MT2.1 : Coastal shrublands and grasslands</t>
         </is>
       </c>
       <c r="B27">
@@ -1317,7 +1317,7 @@
     <row r="28">
       <c r="A28" t="inlineStr">
         <is>
-          <t>MT2.1</t>
+          <t>MT2.1 : Coastal shrublands and grasslands</t>
         </is>
       </c>
       <c r="B28">
@@ -1352,7 +1352,7 @@
     <row r="29">
       <c r="A29" t="inlineStr">
         <is>
-          <t>MT2.1</t>
+          <t>MT2.1 : Coastal shrublands and grasslands</t>
         </is>
       </c>
       <c r="B29">
@@ -1387,7 +1387,7 @@
     <row r="30">
       <c r="A30" t="inlineStr">
         <is>
-          <t>T1.2</t>
+          <t>T1.2 : Tropical-subtropical dry forests and thickets</t>
         </is>
       </c>
       <c r="B30">
@@ -1403,7 +1403,7 @@
         <v>0.9090909090909091</v>
       </c>
       <c r="F30">
-        <v>0.8272727272727273</v>
+        <v>0.8363636363636364</v>
       </c>
       <c r="G30">
         <v>0.9727272727272728</v>
@@ -1422,7 +1422,7 @@
     <row r="31">
       <c r="A31" t="inlineStr">
         <is>
-          <t>T1.2</t>
+          <t>T1.2 : Tropical-subtropical dry forests and thickets</t>
         </is>
       </c>
       <c r="B31">
@@ -1441,7 +1441,7 @@
         <v>0.8090909090909091</v>
       </c>
       <c r="G31">
-        <v>0.9545454545454546</v>
+        <v>0.9636363636363636</v>
       </c>
       <c r="H31" t="inlineStr">
         <is>
@@ -1457,7 +1457,7 @@
     <row r="32">
       <c r="A32" t="inlineStr">
         <is>
-          <t>T1.2</t>
+          <t>T1.2 : Tropical-subtropical dry forests and thickets</t>
         </is>
       </c>
       <c r="B32">
@@ -1492,7 +1492,7 @@
     <row r="33">
       <c r="A33" t="inlineStr">
         <is>
-          <t>T1.2</t>
+          <t>T1.2 : Tropical-subtropical dry forests and thickets</t>
         </is>
       </c>
       <c r="B33">
@@ -1508,7 +1508,7 @@
         <v>0.8909090909090909</v>
       </c>
       <c r="F33">
-        <v>0.8181818181818181</v>
+        <v>0.8090909090909091</v>
       </c>
       <c r="G33">
         <v>0.9636363636363636</v>
@@ -1527,7 +1527,7 @@
     <row r="34">
       <c r="A34" t="inlineStr">
         <is>
-          <t>T2.4</t>
+          <t>T2.4 : Warm temperate laurophyll forests</t>
         </is>
       </c>
       <c r="B34">
@@ -1562,7 +1562,7 @@
     <row r="35">
       <c r="A35" t="inlineStr">
         <is>
-          <t>T2.4</t>
+          <t>T2.4 : Warm temperate laurophyll forests</t>
         </is>
       </c>
       <c r="B35">
@@ -1597,7 +1597,7 @@
     <row r="36">
       <c r="A36" t="inlineStr">
         <is>
-          <t>T2.4</t>
+          <t>T2.4 : Warm temperate laurophyll forests</t>
         </is>
       </c>
       <c r="B36">
@@ -1632,7 +1632,7 @@
     <row r="37">
       <c r="A37" t="inlineStr">
         <is>
-          <t>T2.4</t>
+          <t>T2.4 : Warm temperate laurophyll forests</t>
         </is>
       </c>
       <c r="B37">
@@ -1667,7 +1667,7 @@
     <row r="38">
       <c r="A38" t="inlineStr">
         <is>
-          <t>T3.1</t>
+          <t>T3.1 : Seasonally dry tropical shrublands</t>
         </is>
       </c>
       <c r="B38">
@@ -1702,7 +1702,7 @@
     <row r="39">
       <c r="A39" t="inlineStr">
         <is>
-          <t>T3.1</t>
+          <t>T3.1 : Seasonally dry tropical shrublands</t>
         </is>
       </c>
       <c r="B39">
@@ -1737,7 +1737,7 @@
     <row r="40">
       <c r="A40" t="inlineStr">
         <is>
-          <t>T3.1</t>
+          <t>T3.1 : Seasonally dry tropical shrublands</t>
         </is>
       </c>
       <c r="B40">
@@ -1772,7 +1772,7 @@
     <row r="41">
       <c r="A41" t="inlineStr">
         <is>
-          <t>T3.1</t>
+          <t>T3.1 : Seasonally dry tropical shrublands</t>
         </is>
       </c>
       <c r="B41">
@@ -1807,7 +1807,7 @@
     <row r="42">
       <c r="A42" t="inlineStr">
         <is>
-          <t>T3.2</t>
+          <t>T3.2 : Seasonally dry temperate heaths and shrublands</t>
         </is>
       </c>
       <c r="B42">
@@ -1823,7 +1823,7 @@
         <v>0.6454545454545455</v>
       </c>
       <c r="F42">
-        <v>0.5833333333333333</v>
+        <v>0.5818181818181818</v>
       </c>
       <c r="G42">
         <v>0.7060606060606061</v>
@@ -1842,7 +1842,7 @@
     <row r="43">
       <c r="A43" t="inlineStr">
         <is>
-          <t>T3.2</t>
+          <t>T3.2 : Seasonally dry temperate heaths and shrublands</t>
         </is>
       </c>
       <c r="B43">
@@ -1858,10 +1858,10 @@
         <v>0.6303030303030304</v>
       </c>
       <c r="F43">
-        <v>0.5666666666666667</v>
+        <v>0.5681818181818181</v>
       </c>
       <c r="G43">
-        <v>0.6909090909090909</v>
+        <v>0.693939393939394</v>
       </c>
       <c r="H43" t="inlineStr">
         <is>
@@ -1877,7 +1877,7 @@
     <row r="44">
       <c r="A44" t="inlineStr">
         <is>
-          <t>T3.2</t>
+          <t>T3.2 : Seasonally dry temperate heaths and shrublands</t>
         </is>
       </c>
       <c r="B44">
@@ -1893,7 +1893,7 @@
         <v>0.6303030303030304</v>
       </c>
       <c r="F44">
-        <v>0.5681818181818181</v>
+        <v>0.5666666666666667</v>
       </c>
       <c r="G44">
         <v>0.6909090909090909</v>
@@ -1912,7 +1912,7 @@
     <row r="45">
       <c r="A45" t="inlineStr">
         <is>
-          <t>T3.2</t>
+          <t>T3.2 : Seasonally dry temperate heaths and shrublands</t>
         </is>
       </c>
       <c r="B45">
@@ -1928,10 +1928,10 @@
         <v>0.6303030303030304</v>
       </c>
       <c r="F45">
-        <v>0.5681818181818181</v>
+        <v>0.5666666666666667</v>
       </c>
       <c r="G45">
-        <v>0.6909090909090909</v>
+        <v>0.6924242424242424</v>
       </c>
       <c r="H45" t="inlineStr">
         <is>
@@ -1947,7 +1947,7 @@
     <row r="46">
       <c r="A46" t="inlineStr">
         <is>
-          <t>T4.1</t>
+          <t>T4.1 : Trophic savannas</t>
         </is>
       </c>
       <c r="B46">
@@ -1963,7 +1963,7 @@
         <v>0.9421052631578948</v>
       </c>
       <c r="F46">
-        <v>0.8789473684210526</v>
+        <v>0.8842105263157894</v>
       </c>
       <c r="G46">
         <v>0.9894736842105263</v>
@@ -1982,7 +1982,7 @@
     <row r="47">
       <c r="A47" t="inlineStr">
         <is>
-          <t>T4.1</t>
+          <t>T4.1 : Trophic savannas</t>
         </is>
       </c>
       <c r="B47">
@@ -2017,7 +2017,7 @@
     <row r="48">
       <c r="A48" t="inlineStr">
         <is>
-          <t>T4.1</t>
+          <t>T4.1 : Trophic savannas</t>
         </is>
       </c>
       <c r="B48">
@@ -2052,7 +2052,7 @@
     <row r="49">
       <c r="A49" t="inlineStr">
         <is>
-          <t>T4.1</t>
+          <t>T4.1 : Trophic savannas</t>
         </is>
       </c>
       <c r="B49">
@@ -2087,7 +2087,7 @@
     <row r="50">
       <c r="A50" t="inlineStr">
         <is>
-          <t>T4.2</t>
+          <t>T4.2 : Pyric tussock savannas</t>
         </is>
       </c>
       <c r="B50">
@@ -2103,7 +2103,7 @@
         <v>0.8507462686567164</v>
       </c>
       <c r="F50">
-        <v>0.7850746268656716</v>
+        <v>0.7820895522388059</v>
       </c>
       <c r="G50">
         <v>0.9134328358208955</v>
@@ -2122,7 +2122,7 @@
     <row r="51">
       <c r="A51" t="inlineStr">
         <is>
-          <t>T4.2</t>
+          <t>T4.2 : Pyric tussock savannas</t>
         </is>
       </c>
       <c r="B51">
@@ -2138,10 +2138,10 @@
         <v>0.8149253731343283</v>
       </c>
       <c r="F51">
-        <v>0.7462686567164178</v>
+        <v>0.7432835820895523</v>
       </c>
       <c r="G51">
-        <v>0.8805970149253731</v>
+        <v>0.8835820895522388</v>
       </c>
       <c r="H51" t="inlineStr">
         <is>
@@ -2157,7 +2157,7 @@
     <row r="52">
       <c r="A52" t="inlineStr">
         <is>
-          <t>T4.2</t>
+          <t>T4.2 : Pyric tussock savannas</t>
         </is>
       </c>
       <c r="B52">
@@ -2173,10 +2173,10 @@
         <v>0.8059701492537313</v>
       </c>
       <c r="F52">
-        <v>0.7343283582089553</v>
+        <v>0.7313432835820896</v>
       </c>
       <c r="G52">
-        <v>0.8746268656716418</v>
+        <v>0.8716417910447761</v>
       </c>
       <c r="H52" t="inlineStr">
         <is>
@@ -2192,7 +2192,7 @@
     <row r="53">
       <c r="A53" t="inlineStr">
         <is>
-          <t>T4.2</t>
+          <t>T4.2 : Pyric tussock savannas</t>
         </is>
       </c>
       <c r="B53">
@@ -2208,7 +2208,7 @@
         <v>0.8059701492537313</v>
       </c>
       <c r="F53">
-        <v>0.7343283582089553</v>
+        <v>0.7313432835820896</v>
       </c>
       <c r="G53">
         <v>0.8746268656716418</v>
@@ -2227,7 +2227,7 @@
     <row r="54">
       <c r="A54" t="inlineStr">
         <is>
-          <t>T4.5</t>
+          <t>T4.5 : Temperate subhumid grasslands</t>
         </is>
       </c>
       <c r="B54">
@@ -2262,7 +2262,7 @@
     <row r="55">
       <c r="A55" t="inlineStr">
         <is>
-          <t>T4.5</t>
+          <t>T4.5 : Temperate subhumid grasslands</t>
         </is>
       </c>
       <c r="B55">
@@ -2278,10 +2278,10 @@
         <v>0.8240000000000001</v>
       </c>
       <c r="F55">
-        <v>0.7626666666666666</v>
+        <v>0.76</v>
       </c>
       <c r="G55">
-        <v>0.8853333333333333</v>
+        <v>0.8827333333333324</v>
       </c>
       <c r="H55" t="inlineStr">
         <is>
@@ -2297,7 +2297,7 @@
     <row r="56">
       <c r="A56" t="inlineStr">
         <is>
-          <t>T4.5</t>
+          <t>T4.5 : Temperate subhumid grasslands</t>
         </is>
       </c>
       <c r="B56">
@@ -2313,10 +2313,10 @@
         <v>0.8240000000000001</v>
       </c>
       <c r="F56">
-        <v>0.76</v>
+        <v>0.7573333333333333</v>
       </c>
       <c r="G56">
-        <v>0.8853333333333333</v>
+        <v>0.8826666666666667</v>
       </c>
       <c r="H56" t="inlineStr">
         <is>
@@ -2332,7 +2332,7 @@
     <row r="57">
       <c r="A57" t="inlineStr">
         <is>
-          <t>T4.5</t>
+          <t>T4.5 : Temperate subhumid grasslands</t>
         </is>
       </c>
       <c r="B57">
@@ -2351,7 +2351,7 @@
         <v>0.7493333333333334</v>
       </c>
       <c r="G57">
-        <v>0.8746666666666667</v>
+        <v>0.8773333333333333</v>
       </c>
       <c r="H57" t="inlineStr">
         <is>
@@ -2367,7 +2367,7 @@
     <row r="58">
       <c r="A58" t="inlineStr">
         <is>
-          <t>T5.1</t>
+          <t>T5.1 : Semi-desert steppes</t>
         </is>
       </c>
       <c r="B58">
@@ -2402,7 +2402,7 @@
     <row r="59">
       <c r="A59" t="inlineStr">
         <is>
-          <t>T5.1</t>
+          <t>T5.1 : Semi-desert steppes</t>
         </is>
       </c>
       <c r="B59">
@@ -2437,7 +2437,7 @@
     <row r="60">
       <c r="A60" t="inlineStr">
         <is>
-          <t>T5.1</t>
+          <t>T5.1 : Semi-desert steppes</t>
         </is>
       </c>
       <c r="B60">
@@ -2472,7 +2472,7 @@
     <row r="61">
       <c r="A61" t="inlineStr">
         <is>
-          <t>T5.1</t>
+          <t>T5.1 : Semi-desert steppes</t>
         </is>
       </c>
       <c r="B61">
@@ -2507,7 +2507,7 @@
     <row r="62">
       <c r="A62" t="inlineStr">
         <is>
-          <t>T5.2</t>
+          <t>T5.2 : Thorny deserts and semi-deserts</t>
         </is>
       </c>
       <c r="B62">
@@ -2526,7 +2526,7 @@
         <v>0.8603174603174604</v>
       </c>
       <c r="G62">
-        <v>0.9746031746031746</v>
+        <v>0.9683333333333322</v>
       </c>
       <c r="H62" t="inlineStr">
         <is>
@@ -2542,7 +2542,7 @@
     <row r="63">
       <c r="A63" t="inlineStr">
         <is>
-          <t>T5.2</t>
+          <t>T5.2 : Thorny deserts and semi-deserts</t>
         </is>
       </c>
       <c r="B63">
@@ -2558,7 +2558,7 @@
         <v>0.9079365079365079</v>
       </c>
       <c r="F63">
-        <v>0.8412698412698413</v>
+        <v>0.8444444444444444</v>
       </c>
       <c r="G63">
         <v>0.9650793650793651</v>
@@ -2577,7 +2577,7 @@
     <row r="64">
       <c r="A64" t="inlineStr">
         <is>
-          <t>T5.2</t>
+          <t>T5.2 : Thorny deserts and semi-deserts</t>
         </is>
       </c>
       <c r="B64">
@@ -2612,7 +2612,7 @@
     <row r="65">
       <c r="A65" t="inlineStr">
         <is>
-          <t>T5.2</t>
+          <t>T5.2 : Thorny deserts and semi-deserts</t>
         </is>
       </c>
       <c r="B65">
@@ -2628,7 +2628,7 @@
         <v>0.9079365079365079</v>
       </c>
       <c r="F65">
-        <v>0.8412698412698413</v>
+        <v>0.8475396825396825</v>
       </c>
       <c r="G65">
         <v>0.9650793650793651</v>
@@ -2647,7 +2647,7 @@
     <row r="66">
       <c r="A66" t="inlineStr">
         <is>
-          <t>T5.5</t>
+          <t>T5.5 : Hyper-arid deserts</t>
         </is>
       </c>
       <c r="B66">
@@ -2682,7 +2682,7 @@
     <row r="67">
       <c r="A67" t="inlineStr">
         <is>
-          <t>T5.5</t>
+          <t>T5.5 : Hyper-arid deserts</t>
         </is>
       </c>
       <c r="B67">
@@ -2717,7 +2717,7 @@
     <row r="68">
       <c r="A68" t="inlineStr">
         <is>
-          <t>T5.5</t>
+          <t>T5.5 : Hyper-arid deserts</t>
         </is>
       </c>
       <c r="B68">
@@ -2752,7 +2752,7 @@
     <row r="69">
       <c r="A69" t="inlineStr">
         <is>
-          <t>T5.5</t>
+          <t>T5.5 : Hyper-arid deserts</t>
         </is>
       </c>
       <c r="B69">
@@ -2798,10 +2798,10 @@
         <v>0.8215982721382289</v>
       </c>
       <c r="F70">
-        <v>0.7930885529157667</v>
+        <v>0.7943844492440605</v>
       </c>
       <c r="G70">
-        <v>0.849244060475162</v>
+        <v>0.8475161987041037</v>
       </c>
       <c r="H70" t="inlineStr">
         <is>
@@ -2828,10 +2828,10 @@
         <v>0.7987041036717063</v>
       </c>
       <c r="F71">
-        <v>0.7697624190064795</v>
+        <v>0.770194384449244</v>
       </c>
       <c r="G71">
-        <v>0.8267818574514039</v>
+        <v>0.8272246220302375</v>
       </c>
       <c r="H71" t="inlineStr">
         <is>
@@ -2858,10 +2858,10 @@
         <v>0.7961123110151188</v>
       </c>
       <c r="F72">
-        <v>0.767170626349892</v>
+        <v>0.7680237580993521</v>
       </c>
       <c r="G72">
-        <v>0.8250539956803455</v>
+        <v>0.824622030237581</v>
       </c>
       <c r="H72" t="inlineStr">
         <is>
@@ -2888,10 +2888,10 @@
         <v>0.7943844492440605</v>
       </c>
       <c r="F73">
-        <v>0.7650107991360691</v>
+        <v>0.7641468682505399</v>
       </c>
       <c r="G73">
-        <v>0.8220302375809936</v>
+        <v>0.8237580993520518</v>
       </c>
       <c r="H73" t="inlineStr">
         <is>

</xml_diff>

<commit_message>
added barplot - GET per realm
</commit_message>
<xml_diff>
--- a/data/RLIe_scores.xlsx
+++ b/data/RLIe_scores.xlsx
@@ -407,7 +407,7 @@
     <row r="2">
       <c r="A2" t="inlineStr">
         <is>
-          <t>MT2: Supralittoral coastal systems (n = 10)</t>
+          <t>MT2: Supralittoral coastal systems (n = 10 ecosystems)</t>
         </is>
       </c>
       <c r="B2">
@@ -423,7 +423,7 @@
         <v>0.74</v>
       </c>
       <c r="F2">
-        <v>0.52</v>
+        <v>0.54</v>
       </c>
       <c r="G2">
         <v>0.9399999999999999</v>
@@ -442,7 +442,7 @@
     <row r="3">
       <c r="A3" t="inlineStr">
         <is>
-          <t>MT2: Supralittoral coastal systems (n = 10)</t>
+          <t>MT2: Supralittoral coastal systems (n = 10 ecosystems)</t>
         </is>
       </c>
       <c r="B3">
@@ -461,7 +461,7 @@
         <v>0.34</v>
       </c>
       <c r="G3">
-        <v>0.78</v>
+        <v>0.8</v>
       </c>
       <c r="H3" t="inlineStr">
         <is>
@@ -477,7 +477,7 @@
     <row r="4">
       <c r="A4" t="inlineStr">
         <is>
-          <t>MT2: Supralittoral coastal systems (n = 10)</t>
+          <t>MT2: Supralittoral coastal systems (n = 10 ecosystems)</t>
         </is>
       </c>
       <c r="B4">
@@ -512,7 +512,7 @@
     <row r="5">
       <c r="A5" t="inlineStr">
         <is>
-          <t>MT2: Supralittoral coastal systems (n = 10)</t>
+          <t>MT2: Supralittoral coastal systems (n = 10 ecosystems)</t>
         </is>
       </c>
       <c r="B5">
@@ -547,7 +547,7 @@
     <row r="6">
       <c r="A6" t="inlineStr">
         <is>
-          <t>T1: Tropical-subtropical forests (n = 44)</t>
+          <t>T1: Tropical-subtropical forests (n = 44 ecosystems)</t>
         </is>
       </c>
       <c r="B6">
@@ -582,7 +582,7 @@
     <row r="7">
       <c r="A7" t="inlineStr">
         <is>
-          <t>T1: Tropical-subtropical forests (n = 44)</t>
+          <t>T1: Tropical-subtropical forests (n = 44 ecosystems)</t>
         </is>
       </c>
       <c r="B7">
@@ -601,7 +601,7 @@
         <v>0.8090909090909091</v>
       </c>
       <c r="G7">
-        <v>0.9545454545454546</v>
+        <v>0.9636363636363636</v>
       </c>
       <c r="H7" t="inlineStr">
         <is>
@@ -617,7 +617,7 @@
     <row r="8">
       <c r="A8" t="inlineStr">
         <is>
-          <t>T1: Tropical-subtropical forests (n = 44)</t>
+          <t>T1: Tropical-subtropical forests (n = 44 ecosystems)</t>
         </is>
       </c>
       <c r="B8">
@@ -652,7 +652,7 @@
     <row r="9">
       <c r="A9" t="inlineStr">
         <is>
-          <t>T1: Tropical-subtropical forests (n = 44)</t>
+          <t>T1: Tropical-subtropical forests (n = 44 ecosystems)</t>
         </is>
       </c>
       <c r="B9">
@@ -687,7 +687,7 @@
     <row r="10">
       <c r="A10" t="inlineStr">
         <is>
-          <t>T2: Temperate-boreal forests &amp; woodlands (n = 4)</t>
+          <t>T2: Temperate-boreal forests &amp; woodlands (n = 4 ecosystems)</t>
         </is>
       </c>
       <c r="B10">
@@ -722,7 +722,7 @@
     <row r="11">
       <c r="A11" t="inlineStr">
         <is>
-          <t>T2: Temperate-boreal forests &amp; woodlands (n = 4)</t>
+          <t>T2: Temperate-boreal forests &amp; woodlands (n = 4 ecosystems)</t>
         </is>
       </c>
       <c r="B11">
@@ -757,7 +757,7 @@
     <row r="12">
       <c r="A12" t="inlineStr">
         <is>
-          <t>T2: Temperate-boreal forests &amp; woodlands (n = 4)</t>
+          <t>T2: Temperate-boreal forests &amp; woodlands (n = 4 ecosystems)</t>
         </is>
       </c>
       <c r="B12">
@@ -792,7 +792,7 @@
     <row r="13">
       <c r="A13" t="inlineStr">
         <is>
-          <t>T2: Temperate-boreal forests &amp; woodlands (n = 4)</t>
+          <t>T2: Temperate-boreal forests &amp; woodlands (n = 4 ecosystems)</t>
         </is>
       </c>
       <c r="B13">
@@ -827,7 +827,7 @@
     <row r="14">
       <c r="A14" t="inlineStr">
         <is>
-          <t>T3: Shrublands &amp; shrubby woodlands (n = 133)</t>
+          <t>T3: Shrublands &amp; shrubby woodlands (n = 133 ecosystems)</t>
         </is>
       </c>
       <c r="B14">
@@ -843,10 +843,10 @@
         <v>0.6481203007518797</v>
       </c>
       <c r="F14">
-        <v>0.5864661654135339</v>
+        <v>0.5879323308270676</v>
       </c>
       <c r="G14">
-        <v>0.7082706766917293</v>
+        <v>0.7067669172932332</v>
       </c>
       <c r="H14" t="inlineStr">
         <is>
@@ -862,7 +862,7 @@
     <row r="15">
       <c r="A15" t="inlineStr">
         <is>
-          <t>T3: Shrublands &amp; shrubby woodlands (n = 133)</t>
+          <t>T3: Shrublands &amp; shrubby woodlands (n = 133 ecosystems)</t>
         </is>
       </c>
       <c r="B15">
@@ -878,10 +878,10 @@
         <v>0.6330827067669174</v>
       </c>
       <c r="F15">
-        <v>0.5699248120300752</v>
+        <v>0.5714285714285714</v>
       </c>
       <c r="G15">
-        <v>0.6962406015037594</v>
+        <v>0.6947368421052631</v>
       </c>
       <c r="H15" t="inlineStr">
         <is>
@@ -897,7 +897,7 @@
     <row r="16">
       <c r="A16" t="inlineStr">
         <is>
-          <t>T3: Shrublands &amp; shrubby woodlands (n = 133)</t>
+          <t>T3: Shrublands &amp; shrubby woodlands (n = 133 ecosystems)</t>
         </is>
       </c>
       <c r="B16">
@@ -913,10 +913,10 @@
         <v>0.6330827067669174</v>
       </c>
       <c r="F16">
-        <v>0.5714285714285714</v>
+        <v>0.5698872180451128</v>
       </c>
       <c r="G16">
-        <v>0.6962406015037594</v>
+        <v>0.6947368421052631</v>
       </c>
       <c r="H16" t="inlineStr">
         <is>
@@ -932,7 +932,7 @@
     <row r="17">
       <c r="A17" t="inlineStr">
         <is>
-          <t>T3: Shrublands &amp; shrubby woodlands (n = 133)</t>
+          <t>T3: Shrublands &amp; shrubby woodlands (n = 133 ecosystems)</t>
         </is>
       </c>
       <c r="B17">
@@ -948,10 +948,10 @@
         <v>0.6330827067669174</v>
       </c>
       <c r="F17">
-        <v>0.5714285714285714</v>
+        <v>0.5684210526315789</v>
       </c>
       <c r="G17">
-        <v>0.694774436090225</v>
+        <v>0.6947368421052631</v>
       </c>
       <c r="H17" t="inlineStr">
         <is>
@@ -967,7 +967,7 @@
     <row r="18">
       <c r="A18" t="inlineStr">
         <is>
-          <t>T4: Savannas and grasslands (n = 180)</t>
+          <t>T4: Savannas and grasslands (n = 180 ecosystems)</t>
         </is>
       </c>
       <c r="B18">
@@ -983,7 +983,7 @@
         <v>0.87</v>
       </c>
       <c r="F18">
-        <v>0.8344444444444444</v>
+        <v>0.8333333333333334</v>
       </c>
       <c r="G18">
         <v>0.9055555555555556</v>
@@ -1002,7 +1002,7 @@
     <row r="19">
       <c r="A19" t="inlineStr">
         <is>
-          <t>T4: Savannas and grasslands (n = 180)</t>
+          <t>T4: Savannas and grasslands (n = 180 ecosystems)</t>
         </is>
       </c>
       <c r="B19">
@@ -1018,7 +1018,7 @@
         <v>0.8455555555555556</v>
       </c>
       <c r="F19">
-        <v>0.8066666666666666</v>
+        <v>0.8055555555555556</v>
       </c>
       <c r="G19">
         <v>0.8833333333333333</v>
@@ -1037,7 +1037,7 @@
     <row r="20">
       <c r="A20" t="inlineStr">
         <is>
-          <t>T4: Savannas and grasslands (n = 180)</t>
+          <t>T4: Savannas and grasslands (n = 180 ecosystems)</t>
         </is>
       </c>
       <c r="B20">
@@ -1072,7 +1072,7 @@
     <row r="21">
       <c r="A21" t="inlineStr">
         <is>
-          <t>T4: Savannas and grasslands (n = 180)</t>
+          <t>T4: Savannas and grasslands (n = 180 ecosystems)</t>
         </is>
       </c>
       <c r="B21">
@@ -1091,7 +1091,7 @@
         <v>0.7933333333333333</v>
       </c>
       <c r="G21">
-        <v>0.8733333333333333</v>
+        <v>0.8722499999999996</v>
       </c>
       <c r="H21" t="inlineStr">
         <is>
@@ -1107,7 +1107,7 @@
     <row r="22">
       <c r="A22" t="inlineStr">
         <is>
-          <t>T5: Deserts and semi-deserts (n = 92)</t>
+          <t>T5: Deserts and semi-deserts (n = 92 ecosystems)</t>
         </is>
       </c>
       <c r="B22">
@@ -1123,7 +1123,7 @@
         <v>0.9369565217391305</v>
       </c>
       <c r="F22">
-        <v>0.8891304347826087</v>
+        <v>0.8913043478260869</v>
       </c>
       <c r="G22">
         <v>0.9760869565217392</v>
@@ -1142,7 +1142,7 @@
     <row r="23">
       <c r="A23" t="inlineStr">
         <is>
-          <t>T5: Deserts and semi-deserts (n = 92)</t>
+          <t>T5: Deserts and semi-deserts (n = 92 ecosystems)</t>
         </is>
       </c>
       <c r="B23">
@@ -1158,10 +1158,10 @@
         <v>0.9195652173913044</v>
       </c>
       <c r="F23">
-        <v>0.8673913043478261</v>
+        <v>0.8695652173913043</v>
       </c>
       <c r="G23">
-        <v>0.9652173913043478</v>
+        <v>0.9630434782608696</v>
       </c>
       <c r="H23" t="inlineStr">
         <is>
@@ -1177,7 +1177,7 @@
     <row r="24">
       <c r="A24" t="inlineStr">
         <is>
-          <t>T5: Deserts and semi-deserts (n = 92)</t>
+          <t>T5: Deserts and semi-deserts (n = 92 ecosystems)</t>
         </is>
       </c>
       <c r="B24">
@@ -1212,7 +1212,7 @@
     <row r="25">
       <c r="A25" t="inlineStr">
         <is>
-          <t>T5: Deserts and semi-deserts (n = 92)</t>
+          <t>T5: Deserts and semi-deserts (n = 92 ecosystems)</t>
         </is>
       </c>
       <c r="B25">
@@ -1228,10 +1228,10 @@
         <v>0.9195652173913044</v>
       </c>
       <c r="F25">
-        <v>0.8695652173913043</v>
+        <v>0.8673913043478261</v>
       </c>
       <c r="G25">
-        <v>0.9630434782608696</v>
+        <v>0.9608695652173913</v>
       </c>
       <c r="H25" t="inlineStr">
         <is>
@@ -1247,7 +1247,7 @@
     <row r="26">
       <c r="A26" t="inlineStr">
         <is>
-          <t>MT2.1: Coastal shrublands and grasslands (n = 10)</t>
+          <t>MT2.1: Coastal shrublands and grasslands (n = 10 ecosystems)</t>
         </is>
       </c>
       <c r="B26">
@@ -1282,7 +1282,7 @@
     <row r="27">
       <c r="A27" t="inlineStr">
         <is>
-          <t>MT2.1: Coastal shrublands and grasslands (n = 10)</t>
+          <t>MT2.1: Coastal shrublands and grasslands (n = 10 ecosystems)</t>
         </is>
       </c>
       <c r="B27">
@@ -1317,7 +1317,7 @@
     <row r="28">
       <c r="A28" t="inlineStr">
         <is>
-          <t>MT2.1: Coastal shrublands and grasslands (n = 10)</t>
+          <t>MT2.1: Coastal shrublands and grasslands (n = 10 ecosystems)</t>
         </is>
       </c>
       <c r="B28">
@@ -1352,7 +1352,7 @@
     <row r="29">
       <c r="A29" t="inlineStr">
         <is>
-          <t>MT2.1: Coastal shrublands and grasslands (n = 10)</t>
+          <t>MT2.1: Coastal shrublands and grasslands (n = 10 ecosystems)</t>
         </is>
       </c>
       <c r="B29">
@@ -1387,7 +1387,7 @@
     <row r="30">
       <c r="A30" t="inlineStr">
         <is>
-          <t>T1.2: Tropical-subtropical dry forests and thickets (n = 44)</t>
+          <t>T1.2: Tropical-subtropical dry forests and thickets (n = 44 ecosystems)</t>
         </is>
       </c>
       <c r="B30">
@@ -1422,7 +1422,7 @@
     <row r="31">
       <c r="A31" t="inlineStr">
         <is>
-          <t>T1.2: Tropical-subtropical dry forests and thickets (n = 44)</t>
+          <t>T1.2: Tropical-subtropical dry forests and thickets (n = 44 ecosystems)</t>
         </is>
       </c>
       <c r="B31">
@@ -1457,7 +1457,7 @@
     <row r="32">
       <c r="A32" t="inlineStr">
         <is>
-          <t>T1.2: Tropical-subtropical dry forests and thickets (n = 44)</t>
+          <t>T1.2: Tropical-subtropical dry forests and thickets (n = 44 ecosystems)</t>
         </is>
       </c>
       <c r="B32">
@@ -1492,7 +1492,7 @@
     <row r="33">
       <c r="A33" t="inlineStr">
         <is>
-          <t>T1.2: Tropical-subtropical dry forests and thickets (n = 44)</t>
+          <t>T1.2: Tropical-subtropical dry forests and thickets (n = 44 ecosystems)</t>
         </is>
       </c>
       <c r="B33">
@@ -1527,7 +1527,7 @@
     <row r="34">
       <c r="A34" t="inlineStr">
         <is>
-          <t>T2.4: Warm temperate laurophyll forests (n = 4)</t>
+          <t>T2.4: Warm temperate laurophyll forests (n = 4 ecosystems)</t>
         </is>
       </c>
       <c r="B34">
@@ -1562,7 +1562,7 @@
     <row r="35">
       <c r="A35" t="inlineStr">
         <is>
-          <t>T2.4: Warm temperate laurophyll forests (n = 4)</t>
+          <t>T2.4: Warm temperate laurophyll forests (n = 4 ecosystems)</t>
         </is>
       </c>
       <c r="B35">
@@ -1597,7 +1597,7 @@
     <row r="36">
       <c r="A36" t="inlineStr">
         <is>
-          <t>T2.4: Warm temperate laurophyll forests (n = 4)</t>
+          <t>T2.4: Warm temperate laurophyll forests (n = 4 ecosystems)</t>
         </is>
       </c>
       <c r="B36">
@@ -1632,7 +1632,7 @@
     <row r="37">
       <c r="A37" t="inlineStr">
         <is>
-          <t>T2.4: Warm temperate laurophyll forests (n = 4)</t>
+          <t>T2.4: Warm temperate laurophyll forests (n = 4 ecosystems)</t>
         </is>
       </c>
       <c r="B37">
@@ -1667,7 +1667,7 @@
     <row r="38">
       <c r="A38" t="inlineStr">
         <is>
-          <t>T3.1: Seasonally dry tropical shrublands (n = 1)</t>
+          <t>T3.1: Seasonally dry tropical shrublands (n = 1 ecosystems)</t>
         </is>
       </c>
       <c r="B38">
@@ -1702,7 +1702,7 @@
     <row r="39">
       <c r="A39" t="inlineStr">
         <is>
-          <t>T3.1: Seasonally dry tropical shrublands (n = 1)</t>
+          <t>T3.1: Seasonally dry tropical shrublands (n = 1 ecosystems)</t>
         </is>
       </c>
       <c r="B39">
@@ -1737,7 +1737,7 @@
     <row r="40">
       <c r="A40" t="inlineStr">
         <is>
-          <t>T3.1: Seasonally dry tropical shrublands (n = 1)</t>
+          <t>T3.1: Seasonally dry tropical shrublands (n = 1 ecosystems)</t>
         </is>
       </c>
       <c r="B40">
@@ -1772,7 +1772,7 @@
     <row r="41">
       <c r="A41" t="inlineStr">
         <is>
-          <t>T3.1: Seasonally dry tropical shrublands (n = 1)</t>
+          <t>T3.1: Seasonally dry tropical shrublands (n = 1 ecosystems)</t>
         </is>
       </c>
       <c r="B41">
@@ -1807,7 +1807,7 @@
     <row r="42">
       <c r="A42" t="inlineStr">
         <is>
-          <t>T3.2: Seasonally dry temperate heaths and shrublands (n = 132)</t>
+          <t>T3.2: Seasonally dry temperate heaths and shrublands (n = 132 ecosystems)</t>
         </is>
       </c>
       <c r="B42">
@@ -1826,7 +1826,7 @@
         <v>0.5848484848484848</v>
       </c>
       <c r="G42">
-        <v>0.7075757575757575</v>
+        <v>0.7060984848484843</v>
       </c>
       <c r="H42" t="inlineStr">
         <is>
@@ -1842,7 +1842,7 @@
     <row r="43">
       <c r="A43" t="inlineStr">
         <is>
-          <t>T3.2: Seasonally dry temperate heaths and shrublands (n = 132)</t>
+          <t>T3.2: Seasonally dry temperate heaths and shrublands (n = 132 ecosystems)</t>
         </is>
       </c>
       <c r="B43">
@@ -1861,7 +1861,7 @@
         <v>0.5681818181818181</v>
       </c>
       <c r="G43">
-        <v>0.6924242424242424</v>
+        <v>0.6924621212121206</v>
       </c>
       <c r="H43" t="inlineStr">
         <is>
@@ -1877,7 +1877,7 @@
     <row r="44">
       <c r="A44" t="inlineStr">
         <is>
-          <t>T3.2: Seasonally dry temperate heaths and shrublands (n = 132)</t>
+          <t>T3.2: Seasonally dry temperate heaths and shrublands (n = 132 ecosystems)</t>
         </is>
       </c>
       <c r="B44">
@@ -1912,7 +1912,7 @@
     <row r="45">
       <c r="A45" t="inlineStr">
         <is>
-          <t>T3.2: Seasonally dry temperate heaths and shrublands (n = 132)</t>
+          <t>T3.2: Seasonally dry temperate heaths and shrublands (n = 132 ecosystems)</t>
         </is>
       </c>
       <c r="B45">
@@ -1947,7 +1947,7 @@
     <row r="46">
       <c r="A46" t="inlineStr">
         <is>
-          <t>T4.1: Trophic savannas (n = 38)</t>
+          <t>T4.1: Trophic savannas (n = 38 ecosystems)</t>
         </is>
       </c>
       <c r="B46">
@@ -1963,7 +1963,7 @@
         <v>0.9421052631578948</v>
       </c>
       <c r="F46">
-        <v>0.8842105263157894</v>
+        <v>0.8789473684210526</v>
       </c>
       <c r="G46">
         <v>0.9894736842105263</v>
@@ -1982,7 +1982,7 @@
     <row r="47">
       <c r="A47" t="inlineStr">
         <is>
-          <t>T4.1: Trophic savannas (n = 38)</t>
+          <t>T4.1: Trophic savannas (n = 38 ecosystems)</t>
         </is>
       </c>
       <c r="B47">
@@ -2017,7 +2017,7 @@
     <row r="48">
       <c r="A48" t="inlineStr">
         <is>
-          <t>T4.1: Trophic savannas (n = 38)</t>
+          <t>T4.1: Trophic savannas (n = 38 ecosystems)</t>
         </is>
       </c>
       <c r="B48">
@@ -2052,7 +2052,7 @@
     <row r="49">
       <c r="A49" t="inlineStr">
         <is>
-          <t>T4.1: Trophic savannas (n = 38)</t>
+          <t>T4.1: Trophic savannas (n = 38 ecosystems)</t>
         </is>
       </c>
       <c r="B49">
@@ -2068,7 +2068,7 @@
         <v>0.9263157894736842</v>
       </c>
       <c r="F49">
-        <v>0.8631578947368421</v>
+        <v>0.8578947368421053</v>
       </c>
       <c r="G49">
         <v>0.9842105263157894</v>
@@ -2087,7 +2087,7 @@
     <row r="50">
       <c r="A50" t="inlineStr">
         <is>
-          <t>T4.2: Pyric tussock savannas (n = 67)</t>
+          <t>T4.2: Pyric tussock savannas (n = 67 ecosystems)</t>
         </is>
       </c>
       <c r="B50">
@@ -2122,7 +2122,7 @@
     <row r="51">
       <c r="A51" t="inlineStr">
         <is>
-          <t>T4.2: Pyric tussock savannas (n = 67)</t>
+          <t>T4.2: Pyric tussock savannas (n = 67 ecosystems)</t>
         </is>
       </c>
       <c r="B51">
@@ -2138,10 +2138,10 @@
         <v>0.8149253731343283</v>
       </c>
       <c r="F51">
-        <v>0.7402985074626866</v>
+        <v>0.7432835820895523</v>
       </c>
       <c r="G51">
-        <v>0.8805970149253731</v>
+        <v>0.8835820895522388</v>
       </c>
       <c r="H51" t="inlineStr">
         <is>
@@ -2157,7 +2157,7 @@
     <row r="52">
       <c r="A52" t="inlineStr">
         <is>
-          <t>T4.2: Pyric tussock savannas (n = 67)</t>
+          <t>T4.2: Pyric tussock savannas (n = 67 ecosystems)</t>
         </is>
       </c>
       <c r="B52">
@@ -2192,7 +2192,7 @@
     <row r="53">
       <c r="A53" t="inlineStr">
         <is>
-          <t>T4.2: Pyric tussock savannas (n = 67)</t>
+          <t>T4.2: Pyric tussock savannas (n = 67 ecosystems)</t>
         </is>
       </c>
       <c r="B53">
@@ -2208,10 +2208,10 @@
         <v>0.8059701492537313</v>
       </c>
       <c r="F53">
-        <v>0.7343283582089553</v>
+        <v>0.7313432835820896</v>
       </c>
       <c r="G53">
-        <v>0.8716417910447761</v>
+        <v>0.8746268656716418</v>
       </c>
       <c r="H53" t="inlineStr">
         <is>
@@ -2227,7 +2227,7 @@
     <row r="54">
       <c r="A54" t="inlineStr">
         <is>
-          <t>T4.5: Temperate subhumid grasslands (n = 75)</t>
+          <t>T4.5: Temperate subhumid grasslands (n = 75 ecosystems)</t>
         </is>
       </c>
       <c r="B54">
@@ -2246,7 +2246,7 @@
         <v>0.792</v>
       </c>
       <c r="G54">
-        <v>0.9066666666666666</v>
+        <v>0.904</v>
       </c>
       <c r="H54" t="inlineStr">
         <is>
@@ -2262,7 +2262,7 @@
     <row r="55">
       <c r="A55" t="inlineStr">
         <is>
-          <t>T4.5: Temperate subhumid grasslands (n = 75)</t>
+          <t>T4.5: Temperate subhumid grasslands (n = 75 ecosystems)</t>
         </is>
       </c>
       <c r="B55">
@@ -2278,10 +2278,10 @@
         <v>0.8240000000000001</v>
       </c>
       <c r="F55">
-        <v>0.7599333333333335</v>
+        <v>0.7626666666666666</v>
       </c>
       <c r="G55">
-        <v>0.8826666666666667</v>
+        <v>0.885399999999999</v>
       </c>
       <c r="H55" t="inlineStr">
         <is>
@@ -2297,7 +2297,7 @@
     <row r="56">
       <c r="A56" t="inlineStr">
         <is>
-          <t>T4.5: Temperate subhumid grasslands (n = 75)</t>
+          <t>T4.5: Temperate subhumid grasslands (n = 75 ecosystems)</t>
         </is>
       </c>
       <c r="B56">
@@ -2313,10 +2313,10 @@
         <v>0.8240000000000001</v>
       </c>
       <c r="F56">
-        <v>0.7573333333333333</v>
+        <v>0.7599333333333335</v>
       </c>
       <c r="G56">
-        <v>0.8853333333333333</v>
+        <v>0.8826666666666667</v>
       </c>
       <c r="H56" t="inlineStr">
         <is>
@@ -2332,7 +2332,7 @@
     <row r="57">
       <c r="A57" t="inlineStr">
         <is>
-          <t>T4.5: Temperate subhumid grasslands (n = 75)</t>
+          <t>T4.5: Temperate subhumid grasslands (n = 75 ecosystems)</t>
         </is>
       </c>
       <c r="B57">
@@ -2348,7 +2348,7 @@
         <v>0.8133333333333334</v>
       </c>
       <c r="F57">
-        <v>0.7493333333333334</v>
+        <v>0.7466666666666666</v>
       </c>
       <c r="G57">
         <v>0.8746666666666667</v>
@@ -2367,7 +2367,7 @@
     <row r="58">
       <c r="A58" t="inlineStr">
         <is>
-          <t>T5.1: Semi-desert steppes (n = 15)</t>
+          <t>T5.1: Semi-desert steppes (n = 15 ecosystems)</t>
         </is>
       </c>
       <c r="B58">
@@ -2402,7 +2402,7 @@
     <row r="59">
       <c r="A59" t="inlineStr">
         <is>
-          <t>T5.1: Semi-desert steppes (n = 15)</t>
+          <t>T5.1: Semi-desert steppes (n = 15 ecosystems)</t>
         </is>
       </c>
       <c r="B59">
@@ -2437,7 +2437,7 @@
     <row r="60">
       <c r="A60" t="inlineStr">
         <is>
-          <t>T5.1: Semi-desert steppes (n = 15)</t>
+          <t>T5.1: Semi-desert steppes (n = 15 ecosystems)</t>
         </is>
       </c>
       <c r="B60">
@@ -2472,7 +2472,7 @@
     <row r="61">
       <c r="A61" t="inlineStr">
         <is>
-          <t>T5.1: Semi-desert steppes (n = 15)</t>
+          <t>T5.1: Semi-desert steppes (n = 15 ecosystems)</t>
         </is>
       </c>
       <c r="B61">
@@ -2507,7 +2507,7 @@
     <row r="62">
       <c r="A62" t="inlineStr">
         <is>
-          <t>T5.2: Thorny deserts and semi-deserts (n = 63)</t>
+          <t>T5.2: Thorny deserts and semi-deserts (n = 63 ecosystems)</t>
         </is>
       </c>
       <c r="B62">
@@ -2523,10 +2523,10 @@
         <v>0.9206349206349207</v>
       </c>
       <c r="F62">
-        <v>0.8634920634920635</v>
+        <v>0.8603174603174604</v>
       </c>
       <c r="G62">
-        <v>0.9746031746031746</v>
+        <v>0.9714285714285714</v>
       </c>
       <c r="H62" t="inlineStr">
         <is>
@@ -2542,7 +2542,7 @@
     <row r="63">
       <c r="A63" t="inlineStr">
         <is>
-          <t>T5.2: Thorny deserts and semi-deserts (n = 63)</t>
+          <t>T5.2: Thorny deserts and semi-deserts (n = 63 ecosystems)</t>
         </is>
       </c>
       <c r="B63">
@@ -2561,7 +2561,7 @@
         <v>0.8444444444444444</v>
       </c>
       <c r="G63">
-        <v>0.9650793650793651</v>
+        <v>0.9619047619047619</v>
       </c>
       <c r="H63" t="inlineStr">
         <is>
@@ -2577,7 +2577,7 @@
     <row r="64">
       <c r="A64" t="inlineStr">
         <is>
-          <t>T5.2: Thorny deserts and semi-deserts (n = 63)</t>
+          <t>T5.2: Thorny deserts and semi-deserts (n = 63 ecosystems)</t>
         </is>
       </c>
       <c r="B64">
@@ -2612,7 +2612,7 @@
     <row r="65">
       <c r="A65" t="inlineStr">
         <is>
-          <t>T5.2: Thorny deserts and semi-deserts (n = 63)</t>
+          <t>T5.2: Thorny deserts and semi-deserts (n = 63 ecosystems)</t>
         </is>
       </c>
       <c r="B65">
@@ -2647,7 +2647,7 @@
     <row r="66">
       <c r="A66" t="inlineStr">
         <is>
-          <t>T5.5: Hyper-arid deserts (n = 14)</t>
+          <t>T5.5: Hyper-arid deserts (n = 14 ecosystems)</t>
         </is>
       </c>
       <c r="B66">
@@ -2682,7 +2682,7 @@
     <row r="67">
       <c r="A67" t="inlineStr">
         <is>
-          <t>T5.5: Hyper-arid deserts (n = 14)</t>
+          <t>T5.5: Hyper-arid deserts (n = 14 ecosystems)</t>
         </is>
       </c>
       <c r="B67">
@@ -2717,7 +2717,7 @@
     <row r="68">
       <c r="A68" t="inlineStr">
         <is>
-          <t>T5.5: Hyper-arid deserts (n = 14)</t>
+          <t>T5.5: Hyper-arid deserts (n = 14 ecosystems)</t>
         </is>
       </c>
       <c r="B68">
@@ -2752,7 +2752,7 @@
     <row r="69">
       <c r="A69" t="inlineStr">
         <is>
-          <t>T5.5: Hyper-arid deserts (n = 14)</t>
+          <t>T5.5: Hyper-arid deserts (n = 14 ecosystems)</t>
         </is>
       </c>
       <c r="B69">
@@ -2798,10 +2798,10 @@
         <v>0.8215982721382289</v>
       </c>
       <c r="F70">
-        <v>0.7935205183585313</v>
+        <v>0.7939524838012959</v>
       </c>
       <c r="G70">
-        <v>0.849244060475162</v>
+        <v>0.8483801295896328</v>
       </c>
       <c r="H70" t="inlineStr">
         <is>
@@ -2828,7 +2828,7 @@
         <v>0.7987041036717063</v>
       </c>
       <c r="F71">
-        <v>0.7693304535637149</v>
+        <v>0.7688984881209503</v>
       </c>
       <c r="G71">
         <v>0.8272138228941684</v>
@@ -2858,10 +2858,10 @@
         <v>0.7961123110151188</v>
       </c>
       <c r="F72">
-        <v>0.7658747300215982</v>
+        <v>0.7676025917926566</v>
       </c>
       <c r="G72">
-        <v>0.8237580993520518</v>
+        <v>0.82463282937365</v>
       </c>
       <c r="H72" t="inlineStr">
         <is>
@@ -2888,10 +2888,10 @@
         <v>0.7943844492440605</v>
       </c>
       <c r="F73">
-        <v>0.7650107991360691</v>
+        <v>0.7658747300215982</v>
       </c>
       <c r="G73">
-        <v>0.8241900647948164</v>
+        <v>0.8237580993520518</v>
       </c>
       <c r="H73" t="inlineStr">
         <is>

</xml_diff>

<commit_message>
added RLIE images, finding.qmd and RLE.qmd
</commit_message>
<xml_diff>
--- a/data/RLIe_scores.xlsx
+++ b/data/RLIe_scores.xlsx
@@ -7,7 +7,9 @@
     <workbookView xWindow="240" yWindow="15" windowWidth="16095" windowHeight="9660"/>
   </bookViews>
   <sheets>
-    <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
+    <sheet name="RLIe_GET_L2" sheetId="1" r:id="rId1"/>
+    <sheet name="RLIe_GET_L3" sheetId="2" r:id="rId2"/>
+    <sheet name="RLIe_all" sheetId="3" r:id="rId3"/>
   </sheets>
   <calcPr calcId="124519" fullCalcOnLoad="1"/>
 </workbook>
@@ -351,7 +353,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:I73"/>
+  <dimension ref="A1:I25"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
@@ -461,7 +463,7 @@
         <v>0.34</v>
       </c>
       <c r="G3">
-        <v>0.8</v>
+        <v>0.78</v>
       </c>
       <c r="H3" t="inlineStr">
         <is>
@@ -496,7 +498,7 @@
         <v>0.34</v>
       </c>
       <c r="G4">
-        <v>0.78</v>
+        <v>0.8</v>
       </c>
       <c r="H4" t="inlineStr">
         <is>
@@ -563,7 +565,7 @@
         <v>0.9090909090909091</v>
       </c>
       <c r="F6">
-        <v>0.8272727272727273</v>
+        <v>0.8363636363636364</v>
       </c>
       <c r="G6">
         <v>0.9727272727272728</v>
@@ -843,10 +845,10 @@
         <v>0.6481203007518797</v>
       </c>
       <c r="F14">
-        <v>0.5879323308270676</v>
+        <v>0.58796992481203</v>
       </c>
       <c r="G14">
-        <v>0.7067669172932332</v>
+        <v>0.7082706766917293</v>
       </c>
       <c r="H14" t="inlineStr">
         <is>
@@ -881,7 +883,7 @@
         <v>0.5714285714285714</v>
       </c>
       <c r="G15">
-        <v>0.6947368421052631</v>
+        <v>0.693233082706767</v>
       </c>
       <c r="H15" t="inlineStr">
         <is>
@@ -913,7 +915,7 @@
         <v>0.6330827067669174</v>
       </c>
       <c r="F16">
-        <v>0.5698872180451128</v>
+        <v>0.5699248120300752</v>
       </c>
       <c r="G16">
         <v>0.6947368421052631</v>
@@ -948,10 +950,10 @@
         <v>0.6330827067669174</v>
       </c>
       <c r="F17">
-        <v>0.5684210526315789</v>
+        <v>0.5699248120300752</v>
       </c>
       <c r="G17">
-        <v>0.6947368421052631</v>
+        <v>0.6962406015037594</v>
       </c>
       <c r="H17" t="inlineStr">
         <is>
@@ -983,10 +985,10 @@
         <v>0.87</v>
       </c>
       <c r="F18">
-        <v>0.8333333333333334</v>
+        <v>0.8322222222222222</v>
       </c>
       <c r="G18">
-        <v>0.9055555555555556</v>
+        <v>0.9044444444444444</v>
       </c>
       <c r="H18" t="inlineStr">
         <is>
@@ -1018,7 +1020,7 @@
         <v>0.8455555555555556</v>
       </c>
       <c r="F19">
-        <v>0.8055555555555556</v>
+        <v>0.8066666666666666</v>
       </c>
       <c r="G19">
         <v>0.8833333333333333</v>
@@ -1053,10 +1055,10 @@
         <v>0.8388888888888889</v>
       </c>
       <c r="F20">
-        <v>0.7988888888888889</v>
+        <v>0.8</v>
       </c>
       <c r="G20">
-        <v>0.8766666666666667</v>
+        <v>0.8777777777777778</v>
       </c>
       <c r="H20" t="inlineStr">
         <is>
@@ -1088,10 +1090,10 @@
         <v>0.8344444444444444</v>
       </c>
       <c r="F21">
-        <v>0.7933333333333333</v>
+        <v>0.7944444444444445</v>
       </c>
       <c r="G21">
-        <v>0.8722499999999996</v>
+        <v>0.8733333333333333</v>
       </c>
       <c r="H21" t="inlineStr">
         <is>
@@ -1161,7 +1163,7 @@
         <v>0.8695652173913043</v>
       </c>
       <c r="G23">
-        <v>0.9630434782608696</v>
+        <v>0.9652173913043478</v>
       </c>
       <c r="H23" t="inlineStr">
         <is>
@@ -1196,7 +1198,7 @@
         <v>0.8673913043478261</v>
       </c>
       <c r="G24">
-        <v>0.9630434782608696</v>
+        <v>0.9652173913043478</v>
       </c>
       <c r="H24" t="inlineStr">
         <is>
@@ -1231,7 +1233,7 @@
         <v>0.8673913043478261</v>
       </c>
       <c r="G25">
-        <v>0.9608695652173913</v>
+        <v>0.9630434782608696</v>
       </c>
       <c r="H25" t="inlineStr">
         <is>
@@ -1241,19 +1243,2519 @@
       <c r="I25" t="inlineStr">
         <is>
           <t>GET_L2.count</t>
+        </is>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <dimension ref="A1:I45"/>
+  <sheetViews>
+    <sheetView workbookViewId="0"/>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetData>
+    <row r="1" s="1" customFormat="1">
+      <c r="A1" s="1" t="inlineStr">
+        <is>
+          <t>GET</t>
+        </is>
+      </c>
+      <c r="B1" s="1" t="inlineStr">
+        <is>
+          <t>Year</t>
+        </is>
+      </c>
+      <c r="C1" s="1" t="inlineStr">
+        <is>
+          <t>total_weight</t>
+        </is>
+      </c>
+      <c r="D1" s="1" t="inlineStr">
+        <is>
+          <t>total_count</t>
+        </is>
+      </c>
+      <c r="E1" s="1" t="inlineStr">
+        <is>
+          <t>RLIE</t>
+        </is>
+      </c>
+      <c r="F1" s="1" t="inlineStr">
+        <is>
+          <t>lower</t>
+        </is>
+      </c>
+      <c r="G1" s="1" t="inlineStr">
+        <is>
+          <t>upper</t>
+        </is>
+      </c>
+      <c r="H1" s="1" t="inlineStr">
+        <is>
+          <t>criteria</t>
+        </is>
+      </c>
+      <c r="I1" s="1" t="inlineStr">
+        <is>
+          <t>Analysis_Level</t>
+        </is>
+      </c>
+    </row>
+    <row r="2">
+      <c r="A2" t="inlineStr">
+        <is>
+          <t>MT2.1: Coastal shrublands and grasslands (n = 10 ecosystems)</t>
+        </is>
+      </c>
+      <c r="B2">
+        <v>2014</v>
+      </c>
+      <c r="C2">
+        <v>13</v>
+      </c>
+      <c r="D2">
+        <v>10</v>
+      </c>
+      <c r="E2">
+        <v>0.74</v>
+      </c>
+      <c r="F2">
+        <v>0.54</v>
+      </c>
+      <c r="G2">
+        <v>0.9399999999999999</v>
+      </c>
+      <c r="H2" t="inlineStr">
+        <is>
+          <t>Overall</t>
+        </is>
+      </c>
+      <c r="I2" t="inlineStr">
+        <is>
+          <t>GET_L3.count</t>
+        </is>
+      </c>
+    </row>
+    <row r="3">
+      <c r="A3" t="inlineStr">
+        <is>
+          <t>MT2.1: Coastal shrublands and grasslands (n = 10 ecosystems)</t>
+        </is>
+      </c>
+      <c r="B3">
+        <v>2018</v>
+      </c>
+      <c r="C3">
+        <v>22</v>
+      </c>
+      <c r="D3">
+        <v>10</v>
+      </c>
+      <c r="E3">
+        <v>0.5600000000000001</v>
+      </c>
+      <c r="F3">
+        <v>0.34</v>
+      </c>
+      <c r="G3">
+        <v>0.8</v>
+      </c>
+      <c r="H3" t="inlineStr">
+        <is>
+          <t>Overall</t>
+        </is>
+      </c>
+      <c r="I3" t="inlineStr">
+        <is>
+          <t>GET_L3.count</t>
+        </is>
+      </c>
+    </row>
+    <row r="4">
+      <c r="A4" t="inlineStr">
+        <is>
+          <t>MT2.1: Coastal shrublands and grasslands (n = 10 ecosystems)</t>
+        </is>
+      </c>
+      <c r="B4">
+        <v>2020</v>
+      </c>
+      <c r="C4">
+        <v>22</v>
+      </c>
+      <c r="D4">
+        <v>10</v>
+      </c>
+      <c r="E4">
+        <v>0.5600000000000001</v>
+      </c>
+      <c r="F4">
+        <v>0.34</v>
+      </c>
+      <c r="G4">
+        <v>0.8</v>
+      </c>
+      <c r="H4" t="inlineStr">
+        <is>
+          <t>Overall</t>
+        </is>
+      </c>
+      <c r="I4" t="inlineStr">
+        <is>
+          <t>GET_L3.count</t>
+        </is>
+      </c>
+    </row>
+    <row r="5">
+      <c r="A5" t="inlineStr">
+        <is>
+          <t>MT2.1: Coastal shrublands and grasslands (n = 10 ecosystems)</t>
+        </is>
+      </c>
+      <c r="B5">
+        <v>2024</v>
+      </c>
+      <c r="C5">
+        <v>22</v>
+      </c>
+      <c r="D5">
+        <v>10</v>
+      </c>
+      <c r="E5">
+        <v>0.5600000000000001</v>
+      </c>
+      <c r="F5">
+        <v>0.34</v>
+      </c>
+      <c r="G5">
+        <v>0.78</v>
+      </c>
+      <c r="H5" t="inlineStr">
+        <is>
+          <t>Overall</t>
+        </is>
+      </c>
+      <c r="I5" t="inlineStr">
+        <is>
+          <t>GET_L3.count</t>
+        </is>
+      </c>
+    </row>
+    <row r="6">
+      <c r="A6" t="inlineStr">
+        <is>
+          <t>T1.2: Tropical-subtropical dry forests and thickets (n = 44 ecosystems)</t>
+        </is>
+      </c>
+      <c r="B6">
+        <v>2014</v>
+      </c>
+      <c r="C6">
+        <v>20</v>
+      </c>
+      <c r="D6">
+        <v>44</v>
+      </c>
+      <c r="E6">
+        <v>0.9090909090909091</v>
+      </c>
+      <c r="F6">
+        <v>0.8363636363636364</v>
+      </c>
+      <c r="G6">
+        <v>0.9727272727272728</v>
+      </c>
+      <c r="H6" t="inlineStr">
+        <is>
+          <t>Overall</t>
+        </is>
+      </c>
+      <c r="I6" t="inlineStr">
+        <is>
+          <t>GET_L3.count</t>
+        </is>
+      </c>
+    </row>
+    <row r="7">
+      <c r="A7" t="inlineStr">
+        <is>
+          <t>T1.2: Tropical-subtropical dry forests and thickets (n = 44 ecosystems)</t>
+        </is>
+      </c>
+      <c r="B7">
+        <v>2018</v>
+      </c>
+      <c r="C7">
+        <v>24</v>
+      </c>
+      <c r="D7">
+        <v>44</v>
+      </c>
+      <c r="E7">
+        <v>0.8909090909090909</v>
+      </c>
+      <c r="F7">
+        <v>0.8090909090909091</v>
+      </c>
+      <c r="G7">
+        <v>0.9636363636363636</v>
+      </c>
+      <c r="H7" t="inlineStr">
+        <is>
+          <t>Overall</t>
+        </is>
+      </c>
+      <c r="I7" t="inlineStr">
+        <is>
+          <t>GET_L3.count</t>
+        </is>
+      </c>
+    </row>
+    <row r="8">
+      <c r="A8" t="inlineStr">
+        <is>
+          <t>T1.2: Tropical-subtropical dry forests and thickets (n = 44 ecosystems)</t>
+        </is>
+      </c>
+      <c r="B8">
+        <v>2020</v>
+      </c>
+      <c r="C8">
+        <v>24</v>
+      </c>
+      <c r="D8">
+        <v>44</v>
+      </c>
+      <c r="E8">
+        <v>0.8909090909090909</v>
+      </c>
+      <c r="F8">
+        <v>0.8090909090909091</v>
+      </c>
+      <c r="G8">
+        <v>0.9636363636363636</v>
+      </c>
+      <c r="H8" t="inlineStr">
+        <is>
+          <t>Overall</t>
+        </is>
+      </c>
+      <c r="I8" t="inlineStr">
+        <is>
+          <t>GET_L3.count</t>
+        </is>
+      </c>
+    </row>
+    <row r="9">
+      <c r="A9" t="inlineStr">
+        <is>
+          <t>T1.2: Tropical-subtropical dry forests and thickets (n = 44 ecosystems)</t>
+        </is>
+      </c>
+      <c r="B9">
+        <v>2024</v>
+      </c>
+      <c r="C9">
+        <v>24</v>
+      </c>
+      <c r="D9">
+        <v>44</v>
+      </c>
+      <c r="E9">
+        <v>0.8909090909090909</v>
+      </c>
+      <c r="F9">
+        <v>0.8090909090909091</v>
+      </c>
+      <c r="G9">
+        <v>0.9636363636363636</v>
+      </c>
+      <c r="H9" t="inlineStr">
+        <is>
+          <t>Overall</t>
+        </is>
+      </c>
+      <c r="I9" t="inlineStr">
+        <is>
+          <t>GET_L3.count</t>
+        </is>
+      </c>
+    </row>
+    <row r="10">
+      <c r="A10" t="inlineStr">
+        <is>
+          <t>T2.4: Warm temperate laurophyll forests (n = 4 ecosystems)</t>
+        </is>
+      </c>
+      <c r="B10">
+        <v>2014</v>
+      </c>
+      <c r="C10">
+        <v>0</v>
+      </c>
+      <c r="D10">
+        <v>4</v>
+      </c>
+      <c r="E10">
+        <v>1</v>
+      </c>
+      <c r="F10">
+        <v>1</v>
+      </c>
+      <c r="G10">
+        <v>1</v>
+      </c>
+      <c r="H10" t="inlineStr">
+        <is>
+          <t>Overall</t>
+        </is>
+      </c>
+      <c r="I10" t="inlineStr">
+        <is>
+          <t>GET_L3.count</t>
+        </is>
+      </c>
+    </row>
+    <row r="11">
+      <c r="A11" t="inlineStr">
+        <is>
+          <t>T2.4: Warm temperate laurophyll forests (n = 4 ecosystems)</t>
+        </is>
+      </c>
+      <c r="B11">
+        <v>2018</v>
+      </c>
+      <c r="C11">
+        <v>0</v>
+      </c>
+      <c r="D11">
+        <v>4</v>
+      </c>
+      <c r="E11">
+        <v>1</v>
+      </c>
+      <c r="F11">
+        <v>1</v>
+      </c>
+      <c r="G11">
+        <v>1</v>
+      </c>
+      <c r="H11" t="inlineStr">
+        <is>
+          <t>Overall</t>
+        </is>
+      </c>
+      <c r="I11" t="inlineStr">
+        <is>
+          <t>GET_L3.count</t>
+        </is>
+      </c>
+    </row>
+    <row r="12">
+      <c r="A12" t="inlineStr">
+        <is>
+          <t>T2.4: Warm temperate laurophyll forests (n = 4 ecosystems)</t>
+        </is>
+      </c>
+      <c r="B12">
+        <v>2020</v>
+      </c>
+      <c r="C12">
+        <v>0</v>
+      </c>
+      <c r="D12">
+        <v>4</v>
+      </c>
+      <c r="E12">
+        <v>1</v>
+      </c>
+      <c r="F12">
+        <v>1</v>
+      </c>
+      <c r="G12">
+        <v>1</v>
+      </c>
+      <c r="H12" t="inlineStr">
+        <is>
+          <t>Overall</t>
+        </is>
+      </c>
+      <c r="I12" t="inlineStr">
+        <is>
+          <t>GET_L3.count</t>
+        </is>
+      </c>
+    </row>
+    <row r="13">
+      <c r="A13" t="inlineStr">
+        <is>
+          <t>T2.4: Warm temperate laurophyll forests (n = 4 ecosystems)</t>
+        </is>
+      </c>
+      <c r="B13">
+        <v>2024</v>
+      </c>
+      <c r="C13">
+        <v>0</v>
+      </c>
+      <c r="D13">
+        <v>4</v>
+      </c>
+      <c r="E13">
+        <v>1</v>
+      </c>
+      <c r="F13">
+        <v>1</v>
+      </c>
+      <c r="G13">
+        <v>1</v>
+      </c>
+      <c r="H13" t="inlineStr">
+        <is>
+          <t>Overall</t>
+        </is>
+      </c>
+      <c r="I13" t="inlineStr">
+        <is>
+          <t>GET_L3.count</t>
+        </is>
+      </c>
+    </row>
+    <row r="14">
+      <c r="A14" t="inlineStr">
+        <is>
+          <t>T3.1: Seasonally dry tropical shrublands (n = 1 ecosystems)</t>
+        </is>
+      </c>
+      <c r="B14">
+        <v>2014</v>
+      </c>
+      <c r="C14">
+        <v>0</v>
+      </c>
+      <c r="D14">
+        <v>1</v>
+      </c>
+      <c r="E14">
+        <v>1</v>
+      </c>
+      <c r="F14">
+        <v>1</v>
+      </c>
+      <c r="G14">
+        <v>1</v>
+      </c>
+      <c r="H14" t="inlineStr">
+        <is>
+          <t>Overall</t>
+        </is>
+      </c>
+      <c r="I14" t="inlineStr">
+        <is>
+          <t>GET_L3.count</t>
+        </is>
+      </c>
+    </row>
+    <row r="15">
+      <c r="A15" t="inlineStr">
+        <is>
+          <t>T3.1: Seasonally dry tropical shrublands (n = 1 ecosystems)</t>
+        </is>
+      </c>
+      <c r="B15">
+        <v>2018</v>
+      </c>
+      <c r="C15">
+        <v>0</v>
+      </c>
+      <c r="D15">
+        <v>1</v>
+      </c>
+      <c r="E15">
+        <v>1</v>
+      </c>
+      <c r="F15">
+        <v>1</v>
+      </c>
+      <c r="G15">
+        <v>1</v>
+      </c>
+      <c r="H15" t="inlineStr">
+        <is>
+          <t>Overall</t>
+        </is>
+      </c>
+      <c r="I15" t="inlineStr">
+        <is>
+          <t>GET_L3.count</t>
+        </is>
+      </c>
+    </row>
+    <row r="16">
+      <c r="A16" t="inlineStr">
+        <is>
+          <t>T3.1: Seasonally dry tropical shrublands (n = 1 ecosystems)</t>
+        </is>
+      </c>
+      <c r="B16">
+        <v>2020</v>
+      </c>
+      <c r="C16">
+        <v>0</v>
+      </c>
+      <c r="D16">
+        <v>1</v>
+      </c>
+      <c r="E16">
+        <v>1</v>
+      </c>
+      <c r="F16">
+        <v>1</v>
+      </c>
+      <c r="G16">
+        <v>1</v>
+      </c>
+      <c r="H16" t="inlineStr">
+        <is>
+          <t>Overall</t>
+        </is>
+      </c>
+      <c r="I16" t="inlineStr">
+        <is>
+          <t>GET_L3.count</t>
+        </is>
+      </c>
+    </row>
+    <row r="17">
+      <c r="A17" t="inlineStr">
+        <is>
+          <t>T3.1: Seasonally dry tropical shrublands (n = 1 ecosystems)</t>
+        </is>
+      </c>
+      <c r="B17">
+        <v>2024</v>
+      </c>
+      <c r="C17">
+        <v>0</v>
+      </c>
+      <c r="D17">
+        <v>1</v>
+      </c>
+      <c r="E17">
+        <v>1</v>
+      </c>
+      <c r="F17">
+        <v>1</v>
+      </c>
+      <c r="G17">
+        <v>1</v>
+      </c>
+      <c r="H17" t="inlineStr">
+        <is>
+          <t>Overall</t>
+        </is>
+      </c>
+      <c r="I17" t="inlineStr">
+        <is>
+          <t>GET_L3.count</t>
+        </is>
+      </c>
+    </row>
+    <row r="18">
+      <c r="A18" t="inlineStr">
+        <is>
+          <t>T3.2: Seasonally dry temperate heaths and shrublands (n = 132 ecosystems)</t>
+        </is>
+      </c>
+      <c r="B18">
+        <v>2014</v>
+      </c>
+      <c r="C18">
+        <v>234</v>
+      </c>
+      <c r="D18">
+        <v>132</v>
+      </c>
+      <c r="E18">
+        <v>0.6454545454545455</v>
+      </c>
+      <c r="F18">
+        <v>0.5848484848484848</v>
+      </c>
+      <c r="G18">
+        <v>0.7045454545454546</v>
+      </c>
+      <c r="H18" t="inlineStr">
+        <is>
+          <t>Overall</t>
+        </is>
+      </c>
+      <c r="I18" t="inlineStr">
+        <is>
+          <t>GET_L3.count</t>
+        </is>
+      </c>
+    </row>
+    <row r="19">
+      <c r="A19" t="inlineStr">
+        <is>
+          <t>T3.2: Seasonally dry temperate heaths and shrublands (n = 132 ecosystems)</t>
+        </is>
+      </c>
+      <c r="B19">
+        <v>2018</v>
+      </c>
+      <c r="C19">
+        <v>244</v>
+      </c>
+      <c r="D19">
+        <v>132</v>
+      </c>
+      <c r="E19">
+        <v>0.6303030303030304</v>
+      </c>
+      <c r="F19">
+        <v>0.5666666666666667</v>
+      </c>
+      <c r="G19">
+        <v>0.6909090909090909</v>
+      </c>
+      <c r="H19" t="inlineStr">
+        <is>
+          <t>Overall</t>
+        </is>
+      </c>
+      <c r="I19" t="inlineStr">
+        <is>
+          <t>GET_L3.count</t>
+        </is>
+      </c>
+    </row>
+    <row r="20">
+      <c r="A20" t="inlineStr">
+        <is>
+          <t>T3.2: Seasonally dry temperate heaths and shrublands (n = 132 ecosystems)</t>
+        </is>
+      </c>
+      <c r="B20">
+        <v>2020</v>
+      </c>
+      <c r="C20">
+        <v>244</v>
+      </c>
+      <c r="D20">
+        <v>132</v>
+      </c>
+      <c r="E20">
+        <v>0.6303030303030304</v>
+      </c>
+      <c r="F20">
+        <v>0.5681818181818181</v>
+      </c>
+      <c r="G20">
+        <v>0.6924242424242424</v>
+      </c>
+      <c r="H20" t="inlineStr">
+        <is>
+          <t>Overall</t>
+        </is>
+      </c>
+      <c r="I20" t="inlineStr">
+        <is>
+          <t>GET_L3.count</t>
+        </is>
+      </c>
+    </row>
+    <row r="21">
+      <c r="A21" t="inlineStr">
+        <is>
+          <t>T3.2: Seasonally dry temperate heaths and shrublands (n = 132 ecosystems)</t>
+        </is>
+      </c>
+      <c r="B21">
+        <v>2024</v>
+      </c>
+      <c r="C21">
+        <v>244</v>
+      </c>
+      <c r="D21">
+        <v>132</v>
+      </c>
+      <c r="E21">
+        <v>0.6303030303030304</v>
+      </c>
+      <c r="F21">
+        <v>0.5666666666666667</v>
+      </c>
+      <c r="G21">
+        <v>0.6924242424242424</v>
+      </c>
+      <c r="H21" t="inlineStr">
+        <is>
+          <t>Overall</t>
+        </is>
+      </c>
+      <c r="I21" t="inlineStr">
+        <is>
+          <t>GET_L3.count</t>
+        </is>
+      </c>
+    </row>
+    <row r="22">
+      <c r="A22" t="inlineStr">
+        <is>
+          <t>T4.1: Trophic savannas (n = 38 ecosystems)</t>
+        </is>
+      </c>
+      <c r="B22">
+        <v>2014</v>
+      </c>
+      <c r="C22">
+        <v>11</v>
+      </c>
+      <c r="D22">
+        <v>38</v>
+      </c>
+      <c r="E22">
+        <v>0.9421052631578948</v>
+      </c>
+      <c r="F22">
+        <v>0.8842105263157894</v>
+      </c>
+      <c r="G22">
+        <v>0.9894736842105263</v>
+      </c>
+      <c r="H22" t="inlineStr">
+        <is>
+          <t>Overall</t>
+        </is>
+      </c>
+      <c r="I22" t="inlineStr">
+        <is>
+          <t>GET_L3.count</t>
+        </is>
+      </c>
+    </row>
+    <row r="23">
+      <c r="A23" t="inlineStr">
+        <is>
+          <t>T4.1: Trophic savannas (n = 38 ecosystems)</t>
+        </is>
+      </c>
+      <c r="B23">
+        <v>2018</v>
+      </c>
+      <c r="C23">
+        <v>11</v>
+      </c>
+      <c r="D23">
+        <v>38</v>
+      </c>
+      <c r="E23">
+        <v>0.9421052631578948</v>
+      </c>
+      <c r="F23">
+        <v>0.8842105263157894</v>
+      </c>
+      <c r="G23">
+        <v>0.9894736842105263</v>
+      </c>
+      <c r="H23" t="inlineStr">
+        <is>
+          <t>Overall</t>
+        </is>
+      </c>
+      <c r="I23" t="inlineStr">
+        <is>
+          <t>GET_L3.count</t>
+        </is>
+      </c>
+    </row>
+    <row r="24">
+      <c r="A24" t="inlineStr">
+        <is>
+          <t>T4.1: Trophic savannas (n = 38 ecosystems)</t>
+        </is>
+      </c>
+      <c r="B24">
+        <v>2020</v>
+      </c>
+      <c r="C24">
+        <v>14</v>
+      </c>
+      <c r="D24">
+        <v>38</v>
+      </c>
+      <c r="E24">
+        <v>0.9263157894736842</v>
+      </c>
+      <c r="F24">
+        <v>0.8578947368421053</v>
+      </c>
+      <c r="G24">
+        <v>0.9842105263157894</v>
+      </c>
+      <c r="H24" t="inlineStr">
+        <is>
+          <t>Overall</t>
+        </is>
+      </c>
+      <c r="I24" t="inlineStr">
+        <is>
+          <t>GET_L3.count</t>
+        </is>
+      </c>
+    </row>
+    <row r="25">
+      <c r="A25" t="inlineStr">
+        <is>
+          <t>T4.1: Trophic savannas (n = 38 ecosystems)</t>
+        </is>
+      </c>
+      <c r="B25">
+        <v>2024</v>
+      </c>
+      <c r="C25">
+        <v>14</v>
+      </c>
+      <c r="D25">
+        <v>38</v>
+      </c>
+      <c r="E25">
+        <v>0.9263157894736842</v>
+      </c>
+      <c r="F25">
+        <v>0.8578947368421053</v>
+      </c>
+      <c r="G25">
+        <v>0.9842105263157894</v>
+      </c>
+      <c r="H25" t="inlineStr">
+        <is>
+          <t>Overall</t>
+        </is>
+      </c>
+      <c r="I25" t="inlineStr">
+        <is>
+          <t>GET_L3.count</t>
         </is>
       </c>
     </row>
     <row r="26">
       <c r="A26" t="inlineStr">
         <is>
-          <t>MT2.1: Coastal shrublands and grasslands (n = 10 ecosystems)</t>
+          <t>T4.2: Pyric tussock savannas (n = 67 ecosystems)</t>
         </is>
       </c>
       <c r="B26">
         <v>2014</v>
       </c>
       <c r="C26">
+        <v>50</v>
+      </c>
+      <c r="D26">
+        <v>67</v>
+      </c>
+      <c r="E26">
+        <v>0.8507462686567164</v>
+      </c>
+      <c r="F26">
+        <v>0.7820895522388059</v>
+      </c>
+      <c r="G26">
+        <v>0.9134328358208955</v>
+      </c>
+      <c r="H26" t="inlineStr">
+        <is>
+          <t>Overall</t>
+        </is>
+      </c>
+      <c r="I26" t="inlineStr">
+        <is>
+          <t>GET_L3.count</t>
+        </is>
+      </c>
+    </row>
+    <row r="27">
+      <c r="A27" t="inlineStr">
+        <is>
+          <t>T4.2: Pyric tussock savannas (n = 67 ecosystems)</t>
+        </is>
+      </c>
+      <c r="B27">
+        <v>2018</v>
+      </c>
+      <c r="C27">
+        <v>62</v>
+      </c>
+      <c r="D27">
+        <v>67</v>
+      </c>
+      <c r="E27">
+        <v>0.8149253731343283</v>
+      </c>
+      <c r="F27">
+        <v>0.7462686567164178</v>
+      </c>
+      <c r="G27">
+        <v>0.8805970149253731</v>
+      </c>
+      <c r="H27" t="inlineStr">
+        <is>
+          <t>Overall</t>
+        </is>
+      </c>
+      <c r="I27" t="inlineStr">
+        <is>
+          <t>GET_L3.count</t>
+        </is>
+      </c>
+    </row>
+    <row r="28">
+      <c r="A28" t="inlineStr">
+        <is>
+          <t>T4.2: Pyric tussock savannas (n = 67 ecosystems)</t>
+        </is>
+      </c>
+      <c r="B28">
+        <v>2020</v>
+      </c>
+      <c r="C28">
+        <v>65</v>
+      </c>
+      <c r="D28">
+        <v>67</v>
+      </c>
+      <c r="E28">
+        <v>0.8059701492537313</v>
+      </c>
+      <c r="F28">
+        <v>0.7313432835820896</v>
+      </c>
+      <c r="G28">
+        <v>0.8746268656716418</v>
+      </c>
+      <c r="H28" t="inlineStr">
+        <is>
+          <t>Overall</t>
+        </is>
+      </c>
+      <c r="I28" t="inlineStr">
+        <is>
+          <t>GET_L3.count</t>
+        </is>
+      </c>
+    </row>
+    <row r="29">
+      <c r="A29" t="inlineStr">
+        <is>
+          <t>T4.2: Pyric tussock savannas (n = 67 ecosystems)</t>
+        </is>
+      </c>
+      <c r="B29">
+        <v>2024</v>
+      </c>
+      <c r="C29">
+        <v>65</v>
+      </c>
+      <c r="D29">
+        <v>67</v>
+      </c>
+      <c r="E29">
+        <v>0.8059701492537313</v>
+      </c>
+      <c r="F29">
+        <v>0.7373134328358208</v>
+      </c>
+      <c r="G29">
+        <v>0.8746268656716418</v>
+      </c>
+      <c r="H29" t="inlineStr">
+        <is>
+          <t>Overall</t>
+        </is>
+      </c>
+      <c r="I29" t="inlineStr">
+        <is>
+          <t>GET_L3.count</t>
+        </is>
+      </c>
+    </row>
+    <row r="30">
+      <c r="A30" t="inlineStr">
+        <is>
+          <t>T4.5: Temperate subhumid grasslands (n = 75 ecosystems)</t>
+        </is>
+      </c>
+      <c r="B30">
+        <v>2014</v>
+      </c>
+      <c r="C30">
+        <v>56</v>
+      </c>
+      <c r="D30">
+        <v>75</v>
+      </c>
+      <c r="E30">
+        <v>0.8506666666666667</v>
+      </c>
+      <c r="F30">
+        <v>0.7946666666666666</v>
+      </c>
+      <c r="G30">
+        <v>0.9066666666666666</v>
+      </c>
+      <c r="H30" t="inlineStr">
+        <is>
+          <t>Overall</t>
+        </is>
+      </c>
+      <c r="I30" t="inlineStr">
+        <is>
+          <t>GET_L3.count</t>
+        </is>
+      </c>
+    </row>
+    <row r="31">
+      <c r="A31" t="inlineStr">
+        <is>
+          <t>T4.5: Temperate subhumid grasslands (n = 75 ecosystems)</t>
+        </is>
+      </c>
+      <c r="B31">
+        <v>2018</v>
+      </c>
+      <c r="C31">
+        <v>66</v>
+      </c>
+      <c r="D31">
+        <v>75</v>
+      </c>
+      <c r="E31">
+        <v>0.8240000000000001</v>
+      </c>
+      <c r="F31">
+        <v>0.76</v>
+      </c>
+      <c r="G31">
+        <v>0.8826666666666667</v>
+      </c>
+      <c r="H31" t="inlineStr">
+        <is>
+          <t>Overall</t>
+        </is>
+      </c>
+      <c r="I31" t="inlineStr">
+        <is>
+          <t>GET_L3.count</t>
+        </is>
+      </c>
+    </row>
+    <row r="32">
+      <c r="A32" t="inlineStr">
+        <is>
+          <t>T4.5: Temperate subhumid grasslands (n = 75 ecosystems)</t>
+        </is>
+      </c>
+      <c r="B32">
+        <v>2020</v>
+      </c>
+      <c r="C32">
+        <v>66</v>
+      </c>
+      <c r="D32">
+        <v>75</v>
+      </c>
+      <c r="E32">
+        <v>0.8240000000000001</v>
+      </c>
+      <c r="F32">
+        <v>0.76</v>
+      </c>
+      <c r="G32">
+        <v>0.8826666666666667</v>
+      </c>
+      <c r="H32" t="inlineStr">
+        <is>
+          <t>Overall</t>
+        </is>
+      </c>
+      <c r="I32" t="inlineStr">
+        <is>
+          <t>GET_L3.count</t>
+        </is>
+      </c>
+    </row>
+    <row r="33">
+      <c r="A33" t="inlineStr">
+        <is>
+          <t>T4.5: Temperate subhumid grasslands (n = 75 ecosystems)</t>
+        </is>
+      </c>
+      <c r="B33">
+        <v>2024</v>
+      </c>
+      <c r="C33">
+        <v>70</v>
+      </c>
+      <c r="D33">
+        <v>75</v>
+      </c>
+      <c r="E33">
+        <v>0.8133333333333334</v>
+      </c>
+      <c r="F33">
+        <v>0.7466666666666666</v>
+      </c>
+      <c r="G33">
+        <v>0.8746666666666667</v>
+      </c>
+      <c r="H33" t="inlineStr">
+        <is>
+          <t>Overall</t>
+        </is>
+      </c>
+      <c r="I33" t="inlineStr">
+        <is>
+          <t>GET_L3.count</t>
+        </is>
+      </c>
+    </row>
+    <row r="34">
+      <c r="A34" t="inlineStr">
+        <is>
+          <t>T5.1: Semi-desert steppes (n = 15 ecosystems)</t>
+        </is>
+      </c>
+      <c r="B34">
+        <v>2014</v>
+      </c>
+      <c r="C34">
+        <v>0</v>
+      </c>
+      <c r="D34">
+        <v>15</v>
+      </c>
+      <c r="E34">
+        <v>1</v>
+      </c>
+      <c r="F34">
+        <v>1</v>
+      </c>
+      <c r="G34">
+        <v>1</v>
+      </c>
+      <c r="H34" t="inlineStr">
+        <is>
+          <t>Overall</t>
+        </is>
+      </c>
+      <c r="I34" t="inlineStr">
+        <is>
+          <t>GET_L3.count</t>
+        </is>
+      </c>
+    </row>
+    <row r="35">
+      <c r="A35" t="inlineStr">
+        <is>
+          <t>T5.1: Semi-desert steppes (n = 15 ecosystems)</t>
+        </is>
+      </c>
+      <c r="B35">
+        <v>2018</v>
+      </c>
+      <c r="C35">
+        <v>0</v>
+      </c>
+      <c r="D35">
+        <v>15</v>
+      </c>
+      <c r="E35">
+        <v>1</v>
+      </c>
+      <c r="F35">
+        <v>1</v>
+      </c>
+      <c r="G35">
+        <v>1</v>
+      </c>
+      <c r="H35" t="inlineStr">
+        <is>
+          <t>Overall</t>
+        </is>
+      </c>
+      <c r="I35" t="inlineStr">
+        <is>
+          <t>GET_L3.count</t>
+        </is>
+      </c>
+    </row>
+    <row r="36">
+      <c r="A36" t="inlineStr">
+        <is>
+          <t>T5.1: Semi-desert steppes (n = 15 ecosystems)</t>
+        </is>
+      </c>
+      <c r="B36">
+        <v>2020</v>
+      </c>
+      <c r="C36">
+        <v>0</v>
+      </c>
+      <c r="D36">
+        <v>15</v>
+      </c>
+      <c r="E36">
+        <v>1</v>
+      </c>
+      <c r="F36">
+        <v>1</v>
+      </c>
+      <c r="G36">
+        <v>1</v>
+      </c>
+      <c r="H36" t="inlineStr">
+        <is>
+          <t>Overall</t>
+        </is>
+      </c>
+      <c r="I36" t="inlineStr">
+        <is>
+          <t>GET_L3.count</t>
+        </is>
+      </c>
+    </row>
+    <row r="37">
+      <c r="A37" t="inlineStr">
+        <is>
+          <t>T5.1: Semi-desert steppes (n = 15 ecosystems)</t>
+        </is>
+      </c>
+      <c r="B37">
+        <v>2024</v>
+      </c>
+      <c r="C37">
+        <v>0</v>
+      </c>
+      <c r="D37">
+        <v>15</v>
+      </c>
+      <c r="E37">
+        <v>1</v>
+      </c>
+      <c r="F37">
+        <v>1</v>
+      </c>
+      <c r="G37">
+        <v>1</v>
+      </c>
+      <c r="H37" t="inlineStr">
+        <is>
+          <t>Overall</t>
+        </is>
+      </c>
+      <c r="I37" t="inlineStr">
+        <is>
+          <t>GET_L3.count</t>
+        </is>
+      </c>
+    </row>
+    <row r="38">
+      <c r="A38" t="inlineStr">
+        <is>
+          <t>T5.2: Thorny deserts and semi-deserts (n = 63 ecosystems)</t>
+        </is>
+      </c>
+      <c r="B38">
+        <v>2014</v>
+      </c>
+      <c r="C38">
+        <v>25</v>
+      </c>
+      <c r="D38">
+        <v>63</v>
+      </c>
+      <c r="E38">
+        <v>0.9206349206349207</v>
+      </c>
+      <c r="F38">
+        <v>0.8603174603174604</v>
+      </c>
+      <c r="G38">
+        <v>0.9714285714285714</v>
+      </c>
+      <c r="H38" t="inlineStr">
+        <is>
+          <t>Overall</t>
+        </is>
+      </c>
+      <c r="I38" t="inlineStr">
+        <is>
+          <t>GET_L3.count</t>
+        </is>
+      </c>
+    </row>
+    <row r="39">
+      <c r="A39" t="inlineStr">
+        <is>
+          <t>T5.2: Thorny deserts and semi-deserts (n = 63 ecosystems)</t>
+        </is>
+      </c>
+      <c r="B39">
+        <v>2018</v>
+      </c>
+      <c r="C39">
+        <v>29</v>
+      </c>
+      <c r="D39">
+        <v>63</v>
+      </c>
+      <c r="E39">
+        <v>0.9079365079365079</v>
+      </c>
+      <c r="F39">
+        <v>0.8444444444444444</v>
+      </c>
+      <c r="G39">
+        <v>0.9650793650793651</v>
+      </c>
+      <c r="H39" t="inlineStr">
+        <is>
+          <t>Overall</t>
+        </is>
+      </c>
+      <c r="I39" t="inlineStr">
+        <is>
+          <t>GET_L3.count</t>
+        </is>
+      </c>
+    </row>
+    <row r="40">
+      <c r="A40" t="inlineStr">
+        <is>
+          <t>T5.2: Thorny deserts and semi-deserts (n = 63 ecosystems)</t>
+        </is>
+      </c>
+      <c r="B40">
+        <v>2020</v>
+      </c>
+      <c r="C40">
+        <v>29</v>
+      </c>
+      <c r="D40">
+        <v>63</v>
+      </c>
+      <c r="E40">
+        <v>0.9079365079365079</v>
+      </c>
+      <c r="F40">
+        <v>0.8444444444444444</v>
+      </c>
+      <c r="G40">
+        <v>0.9650793650793651</v>
+      </c>
+      <c r="H40" t="inlineStr">
+        <is>
+          <t>Overall</t>
+        </is>
+      </c>
+      <c r="I40" t="inlineStr">
+        <is>
+          <t>GET_L3.count</t>
+        </is>
+      </c>
+    </row>
+    <row r="41">
+      <c r="A41" t="inlineStr">
+        <is>
+          <t>T5.2: Thorny deserts and semi-deserts (n = 63 ecosystems)</t>
+        </is>
+      </c>
+      <c r="B41">
+        <v>2024</v>
+      </c>
+      <c r="C41">
+        <v>29</v>
+      </c>
+      <c r="D41">
+        <v>63</v>
+      </c>
+      <c r="E41">
+        <v>0.9079365079365079</v>
+      </c>
+      <c r="F41">
+        <v>0.8444444444444444</v>
+      </c>
+      <c r="G41">
+        <v>0.9650793650793651</v>
+      </c>
+      <c r="H41" t="inlineStr">
+        <is>
+          <t>Overall</t>
+        </is>
+      </c>
+      <c r="I41" t="inlineStr">
+        <is>
+          <t>GET_L3.count</t>
+        </is>
+      </c>
+    </row>
+    <row r="42">
+      <c r="A42" t="inlineStr">
+        <is>
+          <t>T5.5: Hyper-arid deserts (n = 14 ecosystems)</t>
+        </is>
+      </c>
+      <c r="B42">
+        <v>2014</v>
+      </c>
+      <c r="C42">
+        <v>4</v>
+      </c>
+      <c r="D42">
+        <v>14</v>
+      </c>
+      <c r="E42">
+        <v>0.9428571428571428</v>
+      </c>
+      <c r="F42">
+        <v>0.8285714285714285</v>
+      </c>
+      <c r="G42">
+        <v>1</v>
+      </c>
+      <c r="H42" t="inlineStr">
+        <is>
+          <t>Overall</t>
+        </is>
+      </c>
+      <c r="I42" t="inlineStr">
+        <is>
+          <t>GET_L3.count</t>
+        </is>
+      </c>
+    </row>
+    <row r="43">
+      <c r="A43" t="inlineStr">
+        <is>
+          <t>T5.5: Hyper-arid deserts (n = 14 ecosystems)</t>
+        </is>
+      </c>
+      <c r="B43">
+        <v>2018</v>
+      </c>
+      <c r="C43">
+        <v>8</v>
+      </c>
+      <c r="D43">
+        <v>14</v>
+      </c>
+      <c r="E43">
+        <v>0.8857142857142857</v>
+      </c>
+      <c r="F43">
+        <v>0.7142857142857143</v>
+      </c>
+      <c r="G43">
+        <v>1</v>
+      </c>
+      <c r="H43" t="inlineStr">
+        <is>
+          <t>Overall</t>
+        </is>
+      </c>
+      <c r="I43" t="inlineStr">
+        <is>
+          <t>GET_L3.count</t>
+        </is>
+      </c>
+    </row>
+    <row r="44">
+      <c r="A44" t="inlineStr">
+        <is>
+          <t>T5.5: Hyper-arid deserts (n = 14 ecosystems)</t>
+        </is>
+      </c>
+      <c r="B44">
+        <v>2020</v>
+      </c>
+      <c r="C44">
+        <v>8</v>
+      </c>
+      <c r="D44">
+        <v>14</v>
+      </c>
+      <c r="E44">
+        <v>0.8857142857142857</v>
+      </c>
+      <c r="F44">
+        <v>0.7142857142857143</v>
+      </c>
+      <c r="G44">
+        <v>1</v>
+      </c>
+      <c r="H44" t="inlineStr">
+        <is>
+          <t>Overall</t>
+        </is>
+      </c>
+      <c r="I44" t="inlineStr">
+        <is>
+          <t>GET_L3.count</t>
+        </is>
+      </c>
+    </row>
+    <row r="45">
+      <c r="A45" t="inlineStr">
+        <is>
+          <t>T5.5: Hyper-arid deserts (n = 14 ecosystems)</t>
+        </is>
+      </c>
+      <c r="B45">
+        <v>2024</v>
+      </c>
+      <c r="C45">
+        <v>8</v>
+      </c>
+      <c r="D45">
+        <v>14</v>
+      </c>
+      <c r="E45">
+        <v>0.8857142857142857</v>
+      </c>
+      <c r="F45">
+        <v>0.7142857142857143</v>
+      </c>
+      <c r="G45">
+        <v>1</v>
+      </c>
+      <c r="H45" t="inlineStr">
+        <is>
+          <t>Overall</t>
+        </is>
+      </c>
+      <c r="I45" t="inlineStr">
+        <is>
+          <t>GET_L3.count</t>
+        </is>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <dimension ref="A1:I73"/>
+  <sheetViews>
+    <sheetView workbookViewId="0"/>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetData>
+    <row r="1" s="1" customFormat="1">
+      <c r="A1" s="1" t="inlineStr">
+        <is>
+          <t>GET</t>
+        </is>
+      </c>
+      <c r="B1" s="1" t="inlineStr">
+        <is>
+          <t>Year</t>
+        </is>
+      </c>
+      <c r="C1" s="1" t="inlineStr">
+        <is>
+          <t>total_weight</t>
+        </is>
+      </c>
+      <c r="D1" s="1" t="inlineStr">
+        <is>
+          <t>total_count</t>
+        </is>
+      </c>
+      <c r="E1" s="1" t="inlineStr">
+        <is>
+          <t>RLIE</t>
+        </is>
+      </c>
+      <c r="F1" s="1" t="inlineStr">
+        <is>
+          <t>lower</t>
+        </is>
+      </c>
+      <c r="G1" s="1" t="inlineStr">
+        <is>
+          <t>upper</t>
+        </is>
+      </c>
+      <c r="H1" s="1" t="inlineStr">
+        <is>
+          <t>criteria</t>
+        </is>
+      </c>
+      <c r="I1" s="1" t="inlineStr">
+        <is>
+          <t>Analysis_Level</t>
+        </is>
+      </c>
+    </row>
+    <row r="2">
+      <c r="A2" t="inlineStr">
+        <is>
+          <t>MT2: Supralittoral coastal systems (n = 10 ecosystems)</t>
+        </is>
+      </c>
+      <c r="B2">
+        <v>2014</v>
+      </c>
+      <c r="C2">
+        <v>13</v>
+      </c>
+      <c r="D2">
+        <v>10</v>
+      </c>
+      <c r="E2">
+        <v>0.74</v>
+      </c>
+      <c r="F2">
+        <v>0.54</v>
+      </c>
+      <c r="G2">
+        <v>0.9399999999999999</v>
+      </c>
+      <c r="H2" t="inlineStr">
+        <is>
+          <t>Overall</t>
+        </is>
+      </c>
+      <c r="I2" t="inlineStr">
+        <is>
+          <t>GET_L2.count</t>
+        </is>
+      </c>
+    </row>
+    <row r="3">
+      <c r="A3" t="inlineStr">
+        <is>
+          <t>MT2: Supralittoral coastal systems (n = 10 ecosystems)</t>
+        </is>
+      </c>
+      <c r="B3">
+        <v>2018</v>
+      </c>
+      <c r="C3">
+        <v>22</v>
+      </c>
+      <c r="D3">
+        <v>10</v>
+      </c>
+      <c r="E3">
+        <v>0.5600000000000001</v>
+      </c>
+      <c r="F3">
+        <v>0.34</v>
+      </c>
+      <c r="G3">
+        <v>0.78</v>
+      </c>
+      <c r="H3" t="inlineStr">
+        <is>
+          <t>Overall</t>
+        </is>
+      </c>
+      <c r="I3" t="inlineStr">
+        <is>
+          <t>GET_L2.count</t>
+        </is>
+      </c>
+    </row>
+    <row r="4">
+      <c r="A4" t="inlineStr">
+        <is>
+          <t>MT2: Supralittoral coastal systems (n = 10 ecosystems)</t>
+        </is>
+      </c>
+      <c r="B4">
+        <v>2020</v>
+      </c>
+      <c r="C4">
+        <v>22</v>
+      </c>
+      <c r="D4">
+        <v>10</v>
+      </c>
+      <c r="E4">
+        <v>0.5600000000000001</v>
+      </c>
+      <c r="F4">
+        <v>0.34</v>
+      </c>
+      <c r="G4">
+        <v>0.8</v>
+      </c>
+      <c r="H4" t="inlineStr">
+        <is>
+          <t>Overall</t>
+        </is>
+      </c>
+      <c r="I4" t="inlineStr">
+        <is>
+          <t>GET_L2.count</t>
+        </is>
+      </c>
+    </row>
+    <row r="5">
+      <c r="A5" t="inlineStr">
+        <is>
+          <t>MT2: Supralittoral coastal systems (n = 10 ecosystems)</t>
+        </is>
+      </c>
+      <c r="B5">
+        <v>2024</v>
+      </c>
+      <c r="C5">
+        <v>22</v>
+      </c>
+      <c r="D5">
+        <v>10</v>
+      </c>
+      <c r="E5">
+        <v>0.5600000000000001</v>
+      </c>
+      <c r="F5">
+        <v>0.34</v>
+      </c>
+      <c r="G5">
+        <v>0.78</v>
+      </c>
+      <c r="H5" t="inlineStr">
+        <is>
+          <t>Overall</t>
+        </is>
+      </c>
+      <c r="I5" t="inlineStr">
+        <is>
+          <t>GET_L2.count</t>
+        </is>
+      </c>
+    </row>
+    <row r="6">
+      <c r="A6" t="inlineStr">
+        <is>
+          <t>T1: Tropical-subtropical forests (n = 44 ecosystems)</t>
+        </is>
+      </c>
+      <c r="B6">
+        <v>2014</v>
+      </c>
+      <c r="C6">
+        <v>20</v>
+      </c>
+      <c r="D6">
+        <v>44</v>
+      </c>
+      <c r="E6">
+        <v>0.9090909090909091</v>
+      </c>
+      <c r="F6">
+        <v>0.8363636363636364</v>
+      </c>
+      <c r="G6">
+        <v>0.9727272727272728</v>
+      </c>
+      <c r="H6" t="inlineStr">
+        <is>
+          <t>Overall</t>
+        </is>
+      </c>
+      <c r="I6" t="inlineStr">
+        <is>
+          <t>GET_L2.count</t>
+        </is>
+      </c>
+    </row>
+    <row r="7">
+      <c r="A7" t="inlineStr">
+        <is>
+          <t>T1: Tropical-subtropical forests (n = 44 ecosystems)</t>
+        </is>
+      </c>
+      <c r="B7">
+        <v>2018</v>
+      </c>
+      <c r="C7">
+        <v>24</v>
+      </c>
+      <c r="D7">
+        <v>44</v>
+      </c>
+      <c r="E7">
+        <v>0.8909090909090909</v>
+      </c>
+      <c r="F7">
+        <v>0.8090909090909091</v>
+      </c>
+      <c r="G7">
+        <v>0.9636363636363636</v>
+      </c>
+      <c r="H7" t="inlineStr">
+        <is>
+          <t>Overall</t>
+        </is>
+      </c>
+      <c r="I7" t="inlineStr">
+        <is>
+          <t>GET_L2.count</t>
+        </is>
+      </c>
+    </row>
+    <row r="8">
+      <c r="A8" t="inlineStr">
+        <is>
+          <t>T1: Tropical-subtropical forests (n = 44 ecosystems)</t>
+        </is>
+      </c>
+      <c r="B8">
+        <v>2020</v>
+      </c>
+      <c r="C8">
+        <v>24</v>
+      </c>
+      <c r="D8">
+        <v>44</v>
+      </c>
+      <c r="E8">
+        <v>0.8909090909090909</v>
+      </c>
+      <c r="F8">
+        <v>0.8090909090909091</v>
+      </c>
+      <c r="G8">
+        <v>0.9636363636363636</v>
+      </c>
+      <c r="H8" t="inlineStr">
+        <is>
+          <t>Overall</t>
+        </is>
+      </c>
+      <c r="I8" t="inlineStr">
+        <is>
+          <t>GET_L2.count</t>
+        </is>
+      </c>
+    </row>
+    <row r="9">
+      <c r="A9" t="inlineStr">
+        <is>
+          <t>T1: Tropical-subtropical forests (n = 44 ecosystems)</t>
+        </is>
+      </c>
+      <c r="B9">
+        <v>2024</v>
+      </c>
+      <c r="C9">
+        <v>24</v>
+      </c>
+      <c r="D9">
+        <v>44</v>
+      </c>
+      <c r="E9">
+        <v>0.8909090909090909</v>
+      </c>
+      <c r="F9">
+        <v>0.8090909090909091</v>
+      </c>
+      <c r="G9">
+        <v>0.9636363636363636</v>
+      </c>
+      <c r="H9" t="inlineStr">
+        <is>
+          <t>Overall</t>
+        </is>
+      </c>
+      <c r="I9" t="inlineStr">
+        <is>
+          <t>GET_L2.count</t>
+        </is>
+      </c>
+    </row>
+    <row r="10">
+      <c r="A10" t="inlineStr">
+        <is>
+          <t>T2: Temperate-boreal forests &amp; woodlands (n = 4 ecosystems)</t>
+        </is>
+      </c>
+      <c r="B10">
+        <v>2014</v>
+      </c>
+      <c r="C10">
+        <v>0</v>
+      </c>
+      <c r="D10">
+        <v>4</v>
+      </c>
+      <c r="E10">
+        <v>1</v>
+      </c>
+      <c r="F10">
+        <v>1</v>
+      </c>
+      <c r="G10">
+        <v>1</v>
+      </c>
+      <c r="H10" t="inlineStr">
+        <is>
+          <t>Overall</t>
+        </is>
+      </c>
+      <c r="I10" t="inlineStr">
+        <is>
+          <t>GET_L2.count</t>
+        </is>
+      </c>
+    </row>
+    <row r="11">
+      <c r="A11" t="inlineStr">
+        <is>
+          <t>T2: Temperate-boreal forests &amp; woodlands (n = 4 ecosystems)</t>
+        </is>
+      </c>
+      <c r="B11">
+        <v>2018</v>
+      </c>
+      <c r="C11">
+        <v>0</v>
+      </c>
+      <c r="D11">
+        <v>4</v>
+      </c>
+      <c r="E11">
+        <v>1</v>
+      </c>
+      <c r="F11">
+        <v>1</v>
+      </c>
+      <c r="G11">
+        <v>1</v>
+      </c>
+      <c r="H11" t="inlineStr">
+        <is>
+          <t>Overall</t>
+        </is>
+      </c>
+      <c r="I11" t="inlineStr">
+        <is>
+          <t>GET_L2.count</t>
+        </is>
+      </c>
+    </row>
+    <row r="12">
+      <c r="A12" t="inlineStr">
+        <is>
+          <t>T2: Temperate-boreal forests &amp; woodlands (n = 4 ecosystems)</t>
+        </is>
+      </c>
+      <c r="B12">
+        <v>2020</v>
+      </c>
+      <c r="C12">
+        <v>0</v>
+      </c>
+      <c r="D12">
+        <v>4</v>
+      </c>
+      <c r="E12">
+        <v>1</v>
+      </c>
+      <c r="F12">
+        <v>1</v>
+      </c>
+      <c r="G12">
+        <v>1</v>
+      </c>
+      <c r="H12" t="inlineStr">
+        <is>
+          <t>Overall</t>
+        </is>
+      </c>
+      <c r="I12" t="inlineStr">
+        <is>
+          <t>GET_L2.count</t>
+        </is>
+      </c>
+    </row>
+    <row r="13">
+      <c r="A13" t="inlineStr">
+        <is>
+          <t>T2: Temperate-boreal forests &amp; woodlands (n = 4 ecosystems)</t>
+        </is>
+      </c>
+      <c r="B13">
+        <v>2024</v>
+      </c>
+      <c r="C13">
+        <v>0</v>
+      </c>
+      <c r="D13">
+        <v>4</v>
+      </c>
+      <c r="E13">
+        <v>1</v>
+      </c>
+      <c r="F13">
+        <v>1</v>
+      </c>
+      <c r="G13">
+        <v>1</v>
+      </c>
+      <c r="H13" t="inlineStr">
+        <is>
+          <t>Overall</t>
+        </is>
+      </c>
+      <c r="I13" t="inlineStr">
+        <is>
+          <t>GET_L2.count</t>
+        </is>
+      </c>
+    </row>
+    <row r="14">
+      <c r="A14" t="inlineStr">
+        <is>
+          <t>T3: Shrublands &amp; shrubby woodlands (n = 133 ecosystems)</t>
+        </is>
+      </c>
+      <c r="B14">
+        <v>2014</v>
+      </c>
+      <c r="C14">
+        <v>234</v>
+      </c>
+      <c r="D14">
+        <v>133</v>
+      </c>
+      <c r="E14">
+        <v>0.6481203007518797</v>
+      </c>
+      <c r="F14">
+        <v>0.58796992481203</v>
+      </c>
+      <c r="G14">
+        <v>0.7082706766917293</v>
+      </c>
+      <c r="H14" t="inlineStr">
+        <is>
+          <t>Overall</t>
+        </is>
+      </c>
+      <c r="I14" t="inlineStr">
+        <is>
+          <t>GET_L2.count</t>
+        </is>
+      </c>
+    </row>
+    <row r="15">
+      <c r="A15" t="inlineStr">
+        <is>
+          <t>T3: Shrublands &amp; shrubby woodlands (n = 133 ecosystems)</t>
+        </is>
+      </c>
+      <c r="B15">
+        <v>2018</v>
+      </c>
+      <c r="C15">
+        <v>244</v>
+      </c>
+      <c r="D15">
+        <v>133</v>
+      </c>
+      <c r="E15">
+        <v>0.6330827067669174</v>
+      </c>
+      <c r="F15">
+        <v>0.5714285714285714</v>
+      </c>
+      <c r="G15">
+        <v>0.693233082706767</v>
+      </c>
+      <c r="H15" t="inlineStr">
+        <is>
+          <t>Overall</t>
+        </is>
+      </c>
+      <c r="I15" t="inlineStr">
+        <is>
+          <t>GET_L2.count</t>
+        </is>
+      </c>
+    </row>
+    <row r="16">
+      <c r="A16" t="inlineStr">
+        <is>
+          <t>T3: Shrublands &amp; shrubby woodlands (n = 133 ecosystems)</t>
+        </is>
+      </c>
+      <c r="B16">
+        <v>2020</v>
+      </c>
+      <c r="C16">
+        <v>244</v>
+      </c>
+      <c r="D16">
+        <v>133</v>
+      </c>
+      <c r="E16">
+        <v>0.6330827067669174</v>
+      </c>
+      <c r="F16">
+        <v>0.5699248120300752</v>
+      </c>
+      <c r="G16">
+        <v>0.6947368421052631</v>
+      </c>
+      <c r="H16" t="inlineStr">
+        <is>
+          <t>Overall</t>
+        </is>
+      </c>
+      <c r="I16" t="inlineStr">
+        <is>
+          <t>GET_L2.count</t>
+        </is>
+      </c>
+    </row>
+    <row r="17">
+      <c r="A17" t="inlineStr">
+        <is>
+          <t>T3: Shrublands &amp; shrubby woodlands (n = 133 ecosystems)</t>
+        </is>
+      </c>
+      <c r="B17">
+        <v>2024</v>
+      </c>
+      <c r="C17">
+        <v>244</v>
+      </c>
+      <c r="D17">
+        <v>133</v>
+      </c>
+      <c r="E17">
+        <v>0.6330827067669174</v>
+      </c>
+      <c r="F17">
+        <v>0.5699248120300752</v>
+      </c>
+      <c r="G17">
+        <v>0.6962406015037594</v>
+      </c>
+      <c r="H17" t="inlineStr">
+        <is>
+          <t>Overall</t>
+        </is>
+      </c>
+      <c r="I17" t="inlineStr">
+        <is>
+          <t>GET_L2.count</t>
+        </is>
+      </c>
+    </row>
+    <row r="18">
+      <c r="A18" t="inlineStr">
+        <is>
+          <t>T4: Savannas and grasslands (n = 180 ecosystems)</t>
+        </is>
+      </c>
+      <c r="B18">
+        <v>2014</v>
+      </c>
+      <c r="C18">
+        <v>117</v>
+      </c>
+      <c r="D18">
+        <v>180</v>
+      </c>
+      <c r="E18">
+        <v>0.87</v>
+      </c>
+      <c r="F18">
+        <v>0.8322222222222222</v>
+      </c>
+      <c r="G18">
+        <v>0.9044444444444444</v>
+      </c>
+      <c r="H18" t="inlineStr">
+        <is>
+          <t>Overall</t>
+        </is>
+      </c>
+      <c r="I18" t="inlineStr">
+        <is>
+          <t>GET_L2.count</t>
+        </is>
+      </c>
+    </row>
+    <row r="19">
+      <c r="A19" t="inlineStr">
+        <is>
+          <t>T4: Savannas and grasslands (n = 180 ecosystems)</t>
+        </is>
+      </c>
+      <c r="B19">
+        <v>2018</v>
+      </c>
+      <c r="C19">
+        <v>139</v>
+      </c>
+      <c r="D19">
+        <v>180</v>
+      </c>
+      <c r="E19">
+        <v>0.8455555555555556</v>
+      </c>
+      <c r="F19">
+        <v>0.8066666666666666</v>
+      </c>
+      <c r="G19">
+        <v>0.8833333333333333</v>
+      </c>
+      <c r="H19" t="inlineStr">
+        <is>
+          <t>Overall</t>
+        </is>
+      </c>
+      <c r="I19" t="inlineStr">
+        <is>
+          <t>GET_L2.count</t>
+        </is>
+      </c>
+    </row>
+    <row r="20">
+      <c r="A20" t="inlineStr">
+        <is>
+          <t>T4: Savannas and grasslands (n = 180 ecosystems)</t>
+        </is>
+      </c>
+      <c r="B20">
+        <v>2020</v>
+      </c>
+      <c r="C20">
+        <v>145</v>
+      </c>
+      <c r="D20">
+        <v>180</v>
+      </c>
+      <c r="E20">
+        <v>0.8388888888888889</v>
+      </c>
+      <c r="F20">
+        <v>0.8</v>
+      </c>
+      <c r="G20">
+        <v>0.8777777777777778</v>
+      </c>
+      <c r="H20" t="inlineStr">
+        <is>
+          <t>Overall</t>
+        </is>
+      </c>
+      <c r="I20" t="inlineStr">
+        <is>
+          <t>GET_L2.count</t>
+        </is>
+      </c>
+    </row>
+    <row r="21">
+      <c r="A21" t="inlineStr">
+        <is>
+          <t>T4: Savannas and grasslands (n = 180 ecosystems)</t>
+        </is>
+      </c>
+      <c r="B21">
+        <v>2024</v>
+      </c>
+      <c r="C21">
+        <v>149</v>
+      </c>
+      <c r="D21">
+        <v>180</v>
+      </c>
+      <c r="E21">
+        <v>0.8344444444444444</v>
+      </c>
+      <c r="F21">
+        <v>0.7944444444444445</v>
+      </c>
+      <c r="G21">
+        <v>0.8733333333333333</v>
+      </c>
+      <c r="H21" t="inlineStr">
+        <is>
+          <t>Overall</t>
+        </is>
+      </c>
+      <c r="I21" t="inlineStr">
+        <is>
+          <t>GET_L2.count</t>
+        </is>
+      </c>
+    </row>
+    <row r="22">
+      <c r="A22" t="inlineStr">
+        <is>
+          <t>T5: Deserts and semi-deserts (n = 92 ecosystems)</t>
+        </is>
+      </c>
+      <c r="B22">
+        <v>2014</v>
+      </c>
+      <c r="C22">
+        <v>29</v>
+      </c>
+      <c r="D22">
+        <v>92</v>
+      </c>
+      <c r="E22">
+        <v>0.9369565217391305</v>
+      </c>
+      <c r="F22">
+        <v>0.8913043478260869</v>
+      </c>
+      <c r="G22">
+        <v>0.9760869565217392</v>
+      </c>
+      <c r="H22" t="inlineStr">
+        <is>
+          <t>Overall</t>
+        </is>
+      </c>
+      <c r="I22" t="inlineStr">
+        <is>
+          <t>GET_L2.count</t>
+        </is>
+      </c>
+    </row>
+    <row r="23">
+      <c r="A23" t="inlineStr">
+        <is>
+          <t>T5: Deserts and semi-deserts (n = 92 ecosystems)</t>
+        </is>
+      </c>
+      <c r="B23">
+        <v>2018</v>
+      </c>
+      <c r="C23">
+        <v>37</v>
+      </c>
+      <c r="D23">
+        <v>92</v>
+      </c>
+      <c r="E23">
+        <v>0.9195652173913044</v>
+      </c>
+      <c r="F23">
+        <v>0.8695652173913043</v>
+      </c>
+      <c r="G23">
+        <v>0.9652173913043478</v>
+      </c>
+      <c r="H23" t="inlineStr">
+        <is>
+          <t>Overall</t>
+        </is>
+      </c>
+      <c r="I23" t="inlineStr">
+        <is>
+          <t>GET_L2.count</t>
+        </is>
+      </c>
+    </row>
+    <row r="24">
+      <c r="A24" t="inlineStr">
+        <is>
+          <t>T5: Deserts and semi-deserts (n = 92 ecosystems)</t>
+        </is>
+      </c>
+      <c r="B24">
+        <v>2020</v>
+      </c>
+      <c r="C24">
+        <v>37</v>
+      </c>
+      <c r="D24">
+        <v>92</v>
+      </c>
+      <c r="E24">
+        <v>0.9195652173913044</v>
+      </c>
+      <c r="F24">
+        <v>0.8673913043478261</v>
+      </c>
+      <c r="G24">
+        <v>0.9652173913043478</v>
+      </c>
+      <c r="H24" t="inlineStr">
+        <is>
+          <t>Overall</t>
+        </is>
+      </c>
+      <c r="I24" t="inlineStr">
+        <is>
+          <t>GET_L2.count</t>
+        </is>
+      </c>
+    </row>
+    <row r="25">
+      <c r="A25" t="inlineStr">
+        <is>
+          <t>T5: Deserts and semi-deserts (n = 92 ecosystems)</t>
+        </is>
+      </c>
+      <c r="B25">
+        <v>2024</v>
+      </c>
+      <c r="C25">
+        <v>37</v>
+      </c>
+      <c r="D25">
+        <v>92</v>
+      </c>
+      <c r="E25">
+        <v>0.9195652173913044</v>
+      </c>
+      <c r="F25">
+        <v>0.8673913043478261</v>
+      </c>
+      <c r="G25">
+        <v>0.9630434782608696</v>
+      </c>
+      <c r="H25" t="inlineStr">
+        <is>
+          <t>Overall</t>
+        </is>
+      </c>
+      <c r="I25" t="inlineStr">
+        <is>
+          <t>GET_L2.count</t>
+        </is>
+      </c>
+    </row>
+    <row r="26">
+      <c r="A26" t="inlineStr">
+        <is>
+          <t>MT2.1: Coastal shrublands and grasslands (n = 10 ecosystems)</t>
+        </is>
+      </c>
+      <c r="B26">
+        <v>2014</v>
+      </c>
+      <c r="C26">
         <v>13</v>
       </c>
       <c r="D26">
@@ -1301,7 +3803,7 @@
         <v>0.34</v>
       </c>
       <c r="G27">
-        <v>0.78</v>
+        <v>0.8</v>
       </c>
       <c r="H27" t="inlineStr">
         <is>
@@ -1336,7 +3838,7 @@
         <v>0.34</v>
       </c>
       <c r="G28">
-        <v>0.78</v>
+        <v>0.8</v>
       </c>
       <c r="H28" t="inlineStr">
         <is>
@@ -1826,7 +4328,7 @@
         <v>0.5848484848484848</v>
       </c>
       <c r="G42">
-        <v>0.7060984848484843</v>
+        <v>0.7045454545454546</v>
       </c>
       <c r="H42" t="inlineStr">
         <is>
@@ -1858,10 +4360,10 @@
         <v>0.6303030303030304</v>
       </c>
       <c r="F43">
-        <v>0.5681818181818181</v>
+        <v>0.5666666666666667</v>
       </c>
       <c r="G43">
-        <v>0.6924621212121206</v>
+        <v>0.6909090909090909</v>
       </c>
       <c r="H43" t="inlineStr">
         <is>
@@ -1893,10 +4395,10 @@
         <v>0.6303030303030304</v>
       </c>
       <c r="F44">
-        <v>0.5696969696969697</v>
+        <v>0.5681818181818181</v>
       </c>
       <c r="G44">
-        <v>0.693939393939394</v>
+        <v>0.6924242424242424</v>
       </c>
       <c r="H44" t="inlineStr">
         <is>
@@ -1928,7 +4430,7 @@
         <v>0.6303030303030304</v>
       </c>
       <c r="F45">
-        <v>0.5681818181818181</v>
+        <v>0.5666666666666667</v>
       </c>
       <c r="G45">
         <v>0.6924242424242424</v>
@@ -1963,7 +4465,7 @@
         <v>0.9421052631578948</v>
       </c>
       <c r="F46">
-        <v>0.8789473684210526</v>
+        <v>0.8842105263157894</v>
       </c>
       <c r="G46">
         <v>0.9894736842105263</v>
@@ -2033,7 +4535,7 @@
         <v>0.9263157894736842</v>
       </c>
       <c r="F48">
-        <v>0.8631578947368421</v>
+        <v>0.8578947368421053</v>
       </c>
       <c r="G48">
         <v>0.9842105263157894</v>
@@ -2138,10 +4640,10 @@
         <v>0.8149253731343283</v>
       </c>
       <c r="F51">
-        <v>0.7432835820895523</v>
+        <v>0.7462686567164178</v>
       </c>
       <c r="G51">
-        <v>0.8835820895522388</v>
+        <v>0.8805970149253731</v>
       </c>
       <c r="H51" t="inlineStr">
         <is>
@@ -2173,7 +4675,7 @@
         <v>0.8059701492537313</v>
       </c>
       <c r="F52">
-        <v>0.7343283582089553</v>
+        <v>0.7313432835820896</v>
       </c>
       <c r="G52">
         <v>0.8746268656716418</v>
@@ -2208,7 +4710,7 @@
         <v>0.8059701492537313</v>
       </c>
       <c r="F53">
-        <v>0.7313432835820896</v>
+        <v>0.7373134328358208</v>
       </c>
       <c r="G53">
         <v>0.8746268656716418</v>
@@ -2243,10 +4745,10 @@
         <v>0.8506666666666667</v>
       </c>
       <c r="F54">
-        <v>0.792</v>
+        <v>0.7946666666666666</v>
       </c>
       <c r="G54">
-        <v>0.904</v>
+        <v>0.9066666666666666</v>
       </c>
       <c r="H54" t="inlineStr">
         <is>
@@ -2278,10 +4780,10 @@
         <v>0.8240000000000001</v>
       </c>
       <c r="F55">
-        <v>0.7626666666666666</v>
+        <v>0.76</v>
       </c>
       <c r="G55">
-        <v>0.885399999999999</v>
+        <v>0.8826666666666667</v>
       </c>
       <c r="H55" t="inlineStr">
         <is>
@@ -2313,7 +4815,7 @@
         <v>0.8240000000000001</v>
       </c>
       <c r="F56">
-        <v>0.7599333333333335</v>
+        <v>0.76</v>
       </c>
       <c r="G56">
         <v>0.8826666666666667</v>
@@ -2561,7 +5063,7 @@
         <v>0.8444444444444444</v>
       </c>
       <c r="G63">
-        <v>0.9619047619047619</v>
+        <v>0.9650793650793651</v>
       </c>
       <c r="H63" t="inlineStr">
         <is>
@@ -2593,7 +5095,7 @@
         <v>0.9079365079365079</v>
       </c>
       <c r="F64">
-        <v>0.8412698412698413</v>
+        <v>0.8444444444444444</v>
       </c>
       <c r="G64">
         <v>0.9650793650793651</v>
@@ -2628,7 +5130,7 @@
         <v>0.9079365079365079</v>
       </c>
       <c r="F65">
-        <v>0.8476190476190476</v>
+        <v>0.8444444444444444</v>
       </c>
       <c r="G65">
         <v>0.9650793650793651</v>
@@ -2798,10 +5300,10 @@
         <v>0.8215982721382289</v>
       </c>
       <c r="F70">
-        <v>0.7939524838012959</v>
+        <v>0.7943844492440605</v>
       </c>
       <c r="G70">
-        <v>0.8483801295896328</v>
+        <v>0.849244060475162</v>
       </c>
       <c r="H70" t="inlineStr">
         <is>
@@ -2828,10 +5330,10 @@
         <v>0.7987041036717063</v>
       </c>
       <c r="F71">
-        <v>0.7688984881209503</v>
+        <v>0.7693304535637149</v>
       </c>
       <c r="G71">
-        <v>0.8272138228941684</v>
+        <v>0.8267818574514039</v>
       </c>
       <c r="H71" t="inlineStr">
         <is>
@@ -2861,7 +5363,7 @@
         <v>0.7676025917926566</v>
       </c>
       <c r="G72">
-        <v>0.82463282937365</v>
+        <v>0.8250539956803455</v>
       </c>
       <c r="H72" t="inlineStr">
         <is>
@@ -2888,10 +5390,10 @@
         <v>0.7943844492440605</v>
       </c>
       <c r="F73">
-        <v>0.7658747300215982</v>
+        <v>0.7649999999999999</v>
       </c>
       <c r="G73">
-        <v>0.8237580993520518</v>
+        <v>0.8233261339092872</v>
       </c>
       <c r="H73" t="inlineStr">
         <is>

</xml_diff>